<commit_message>
2  files moved towards a particular folder
2  files moved towards a particular folder
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Marketing/AI marketing/AI Workshop Schools.xlsx
+++ b/Offline/BusinessManagement/Marketing/AI marketing/AI Workshop Schools.xlsx
@@ -1,18 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Marketing\AI marketing\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE224C0D-941E-42D5-8920-34F8307A300E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="540"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="School-Details" sheetId="7" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="8" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,12 +26,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>del</author>
   </authors>
   <commentList>
-    <comment ref="G1" authorId="0" shapeId="0">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -58,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="241">
   <si>
     <t>CBSE</t>
   </si>
@@ -789,8 +791,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -852,16 +854,37 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="26"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -869,12 +892,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -902,6 +940,16 @@
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1182,11 +1230,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K152"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E123" sqref="E123"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B203" sqref="B203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1387,6 +1435,9 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="A14" s="4">
+        <v>13</v>
+      </c>
       <c r="B14" s="3" t="s">
         <v>57</v>
       </c>
@@ -1396,7 +1447,7 @@
     </row>
     <row r="15" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>55</v>
@@ -1407,7 +1458,7 @@
     </row>
     <row r="16" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>21</v>
@@ -1418,7 +1469,7 @@
     </row>
     <row r="17" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>22</v>
@@ -1429,7 +1480,7 @@
     </row>
     <row r="18" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>23</v>
@@ -1440,7 +1491,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>24</v>
@@ -1451,7 +1502,7 @@
     </row>
     <row r="20" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>25</v>
@@ -1465,7 +1516,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>27</v>
@@ -1479,7 +1530,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>28</v>
@@ -1493,7 +1544,7 @@
     </row>
     <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>29</v>
@@ -1507,7 +1558,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>30</v>
@@ -1521,7 +1572,7 @@
     </row>
     <row r="25" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>31</v>
@@ -1535,7 +1586,7 @@
     </row>
     <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>32</v>
@@ -1549,7 +1600,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>33</v>
@@ -1563,7 +1614,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>34</v>
@@ -1574,7 +1625,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>75</v>
@@ -1585,7 +1636,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>35</v>
@@ -1599,7 +1650,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>39</v>
@@ -1613,7 +1664,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>40</v>
@@ -1627,7 +1678,7 @@
     </row>
     <row r="33" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>79</v>
@@ -1644,7 +1695,7 @@
     </row>
     <row r="34" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>82</v>
@@ -1658,7 +1709,7 @@
     </row>
     <row r="35" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>83</v>
@@ -1675,7 +1726,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>85</v>
@@ -1692,7 +1743,7 @@
     </row>
     <row r="37" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>88</v>
@@ -1709,7 +1760,7 @@
     </row>
     <row r="38" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>90</v>
@@ -1723,7 +1774,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>91</v>
@@ -1734,7 +1785,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>92</v>
@@ -1748,7 +1799,7 @@
     </row>
     <row r="41" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>93</v>
@@ -1765,7 +1816,7 @@
     </row>
     <row r="42" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="4">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>95</v>
@@ -1782,7 +1833,7 @@
     </row>
     <row r="43" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>97</v>
@@ -1799,7 +1850,7 @@
     </row>
     <row r="44" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>99</v>
@@ -1813,7 +1864,7 @@
     </row>
     <row r="45" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A45" s="4">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>100</v>
@@ -1827,7 +1878,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="4">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>101</v>
@@ -1838,7 +1889,7 @@
     </row>
     <row r="47" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" s="4">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>102</v>
@@ -1855,7 +1906,7 @@
     </row>
     <row r="48" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>105</v>
@@ -1872,7 +1923,7 @@
     </row>
     <row r="49" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" s="4">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>107</v>
@@ -1889,7 +1940,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="4">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>109</v>
@@ -1906,7 +1957,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="4">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>111</v>
@@ -1923,7 +1974,7 @@
     </row>
     <row r="52" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A52" s="4">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>113</v>
@@ -1940,7 +1991,7 @@
     </row>
     <row r="53" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" s="4">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>115</v>
@@ -1957,7 +2008,7 @@
     </row>
     <row r="54" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A54" s="4">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>117</v>
@@ -1974,7 +2025,7 @@
     </row>
     <row r="55" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A55" s="4">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>119</v>
@@ -1991,7 +2042,7 @@
     </row>
     <row r="56" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A56" s="4">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>121</v>
@@ -2008,7 +2059,7 @@
     </row>
     <row r="57" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A57" s="4">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>123</v>
@@ -2025,7 +2076,7 @@
     </row>
     <row r="58" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A58" s="4">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>123</v>
@@ -2042,7 +2093,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="4">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>125</v>
@@ -2059,7 +2110,7 @@
     </row>
     <row r="60" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A60" s="4">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>127</v>
@@ -2076,7 +2127,7 @@
     </row>
     <row r="61" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A61" s="4">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>130</v>
@@ -2093,7 +2144,7 @@
     </row>
     <row r="62" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A62" s="4">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>132</v>
@@ -2110,7 +2161,7 @@
     </row>
     <row r="63" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A63" s="4">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>134</v>
@@ -2127,7 +2178,7 @@
     </row>
     <row r="64" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A64" s="4">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>137</v>
@@ -2144,7 +2195,7 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="4">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>139</v>
@@ -2161,7 +2212,7 @@
     </row>
     <row r="66" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A66" s="4">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>141</v>
@@ -2178,7 +2229,7 @@
     </row>
     <row r="67" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A67" s="4">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>143</v>
@@ -2195,7 +2246,7 @@
     </row>
     <row r="68" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A68" s="4">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>145</v>
@@ -2212,7 +2263,7 @@
     </row>
     <row r="69" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A69" s="4">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>147</v>
@@ -2229,7 +2280,7 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="4">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>149</v>
@@ -2246,7 +2297,7 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="4">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>151</v>
@@ -2263,7 +2314,7 @@
     </row>
     <row r="72" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A72" s="4">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>153</v>
@@ -2280,7 +2331,7 @@
     </row>
     <row r="73" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A73" s="4">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>155</v>
@@ -2297,7 +2348,7 @@
     </row>
     <row r="74" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A74" s="4">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>157</v>
@@ -2311,7 +2362,7 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="4">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>158</v>
@@ -2328,7 +2379,7 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="4">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>160</v>
@@ -2342,7 +2393,7 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="4">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>161</v>
@@ -2353,7 +2404,7 @@
     </row>
     <row r="78" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="4">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>162</v>
@@ -2370,7 +2421,7 @@
     </row>
     <row r="79" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="4">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>164</v>
@@ -2387,7 +2438,7 @@
     </row>
     <row r="80" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="4">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>166</v>
@@ -2404,7 +2455,7 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="4">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>168</v>
@@ -2421,7 +2472,7 @@
     </row>
     <row r="82" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A82" s="4">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>170</v>
@@ -2435,7 +2486,7 @@
     </row>
     <row r="83" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A83" s="4">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B83" s="3" t="s">
         <v>172</v>
@@ -2449,7 +2500,7 @@
     </row>
     <row r="84" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="4">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B84" s="3" t="s">
         <v>174</v>
@@ -2463,7 +2514,7 @@
     </row>
     <row r="85" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="4">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>175</v>
@@ -2480,7 +2531,7 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" s="4">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B86" s="3" t="s">
         <v>177</v>
@@ -2494,7 +2545,7 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" s="4">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>178</v>
@@ -2508,7 +2559,7 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" s="4">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>179</v>
@@ -2525,7 +2576,7 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" s="4">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>181</v>
@@ -2542,7 +2593,7 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" s="4">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B90" s="3" t="s">
         <v>183</v>
@@ -2556,7 +2607,7 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" s="4">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B91" s="3" t="s">
         <v>184</v>
@@ -2573,7 +2624,7 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" s="4">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>186</v>
@@ -2587,7 +2638,7 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" s="4">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>187</v>
@@ -2601,7 +2652,7 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" s="4">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B94" s="3" t="s">
         <v>188</v>
@@ -2615,7 +2666,7 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" s="4">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B95" s="3" t="s">
         <v>189</v>
@@ -2629,7 +2680,7 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" s="4">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B96" s="3" t="s">
         <v>190</v>
@@ -2643,7 +2694,7 @@
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A97" s="4">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B97" s="3" t="s">
         <v>192</v>
@@ -2657,7 +2708,7 @@
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A98" s="4">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B98" s="3" t="s">
         <v>193</v>
@@ -2668,7 +2719,7 @@
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A99" s="4">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B99" s="3" t="s">
         <v>194</v>
@@ -2679,7 +2730,7 @@
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A100" s="4">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>195</v>
@@ -2690,7 +2741,7 @@
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A101" s="4">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B101" s="3" t="s">
         <v>202</v>
@@ -2701,7 +2752,7 @@
     </row>
     <row r="102" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A102" s="4">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B102" s="3" t="s">
         <v>203</v>
@@ -2712,7 +2763,7 @@
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A103" s="4">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B103" s="3" t="s">
         <v>24</v>
@@ -2723,7 +2774,7 @@
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A104" s="4">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>196</v>
@@ -2734,7 +2785,7 @@
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A105" s="4">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B105" s="3" t="s">
         <v>197</v>
@@ -2745,7 +2796,7 @@
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A106" s="4">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B106" s="3" t="s">
         <v>198</v>
@@ -2755,8 +2806,8 @@
       </c>
     </row>
     <row r="107" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A107" s="2">
-        <v>105</v>
+      <c r="A107" s="4">
+        <v>106</v>
       </c>
       <c r="B107" s="3" t="s">
         <v>199</v>
@@ -2767,7 +2818,7 @@
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A108" s="4">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B108" s="3" t="s">
         <v>210</v>
@@ -2778,7 +2829,7 @@
     </row>
     <row r="109" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A109" s="4">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B109" s="3" t="s">
         <v>212</v>
@@ -2789,7 +2840,7 @@
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A110" s="4">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B110" s="3" t="s">
         <v>215</v>
@@ -2800,7 +2851,7 @@
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A111" s="4">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B111" s="3" t="s">
         <v>217</v>
@@ -2811,7 +2862,7 @@
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A112" s="4">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B112" s="3" t="s">
         <v>219</v>
@@ -2822,7 +2873,7 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" s="4">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B113" s="3" t="s">
         <v>221</v>
@@ -2833,7 +2884,7 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" s="4">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B114" s="3" t="s">
         <v>223</v>
@@ -2844,7 +2895,7 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" s="4">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B115" s="3" t="s">
         <v>225</v>
@@ -2855,7 +2906,7 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" s="4">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B116" s="3" t="s">
         <v>227</v>
@@ -2866,7 +2917,7 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" s="4">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B117" s="3" t="s">
         <v>229</v>
@@ -2877,7 +2928,7 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" s="4">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B118" s="3" t="s">
         <v>231</v>
@@ -2888,7 +2939,7 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" s="4">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B119" s="3" t="s">
         <v>234</v>
@@ -2899,7 +2950,7 @@
     </row>
     <row r="120" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A120" s="4">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B120" s="3" t="s">
         <v>235</v>
@@ -2910,7 +2961,7 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" s="4">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B121" s="3" t="s">
         <v>237</v>
@@ -2921,7 +2972,7 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" s="4">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B122" s="3" t="s">
         <v>239</v>
@@ -2932,209 +2983,1449 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" s="4">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" s="4">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" s="4">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" s="4">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" s="4">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" s="4">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A129" s="4">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A130" s="4">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A131" s="4">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A132" s="4">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A133" s="4">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A134" s="4">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A135" s="4">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A136" s="4">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A137" s="4">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A138" s="4">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A139" s="4">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A140" s="4">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A141" s="4">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A142" s="4">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A143" s="4">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A144" s="4">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A145" s="4">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A146" s="4">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A147" s="4">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A148" s="4">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A149" s="4">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A150" s="4">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A151" s="4">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A152" s="4">
-        <v>150</v>
+        <v>151</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A153" s="4">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A154" s="4">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A155" s="4">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A156" s="4">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A157" s="4">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A158" s="4">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A159" s="4">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A160" s="4">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A161" s="4">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A162" s="4">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A163" s="4">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A164" s="4">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A165" s="4">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A166" s="4">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A167" s="4">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A168" s="4">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A169" s="4">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A170" s="4">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A171" s="4">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A172" s="4">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A173" s="4">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A174" s="4">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A175" s="4">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A176" s="4">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A177" s="4">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A178" s="4">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A179" s="4">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A180" s="4">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A181" s="4">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A182" s="4">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A183" s="4">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A184" s="4">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A185" s="4">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A186" s="4">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A187" s="4">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A188" s="4">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A189" s="4">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A190" s="4">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A191" s="4">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A192" s="4">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A193" s="4">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A194" s="4">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A195" s="4">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A196" s="4">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A197" s="4">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A198" s="4">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A199" s="4">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A200" s="4">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A201" s="4">
+        <v>200</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D31" r:id="rId1"/>
-    <hyperlink ref="D32" r:id="rId2"/>
-    <hyperlink ref="E7" r:id="rId3" display="https://www.google.com/search?q=panchasayar+siksha+niketan&amp;sca_esv=593615924&amp;rlz=1C1CHBF_enAU1047AU1047&amp;sxsrf=AM9HkKnlKkWvrpmDIvMzNnJR8ZC_8s6gNQ%3A1703524925488&amp;ei=PbqJZaauHY2KnesPo--TuAo&amp;gs_ssp=eJzj4tFP1zc0MqnMzTa1TDNgtFI1qDBONDAyNzRPNU1LM0xOTkuyAgqZpJmZmJgnGZgZGSWnpSV5SRUk5iVnJBYnViYWKRRnZhdnJCrkZWanliTmAQC7Qxln&amp;oq=panchasayar+s&amp;gs_lp=Egxnd3Mtd2l6LXNlcnAiDXBhbmNoYXNheWFyIHMqAggAMhQQLhivARjHARimAxioAxiABBiOBTIFEAAYgAQyBRAAGIAEMgsQLhiABBioAxidAzIFEAAYgAQyBRAAGIAEMgUQABiABDIFEAAYgAQyCBAAGIAEGMsBMggQABiABBjLATIjEC4YrwEYxwEYpgMYqAMYgAQYjgUYlwUY3AQY3gQY4ATYAQNIuzhQmhhYmCVwAXgBkAEAmAGvAqAB1gSqAQUyLTEuMbgBAcgBAPgBAcICChAAGEcY1gQYsAPCAg0QABiABBiKBRhDGLADwgIcEC4YgAQYigUYQxjHARivARjIAxiwAxiOBdgBAcICGRAuGIAEGIoFGEMYxwEYrwEYyAMYsAPYAQHCAg4QABjkAhjWBBiwA9gBAsICEBAuGEMYnQMYqAMYgAQYigXCAhAQLhiABBiKBRhDGKgDGJ0DwgIWEC4YQxivARjHARimAxioAxiABBiKBcICChAAGIAEGBQYhwLCAh8QLhhDGJ0DGKgDGIAEGIoFGJcFGNwEGN4EGOAE2AED4gMEGAAgQYgGAZAGDroGBggBEAEYCLoGBggCEAEYCboGBggDEAEYFA&amp;sclient=gws-wiz-serp"/>
-    <hyperlink ref="E8" r:id="rId4" display="https://www.google.com/search?q=miranda+high+school&amp;sca_esv=593615924&amp;rlz=1C1CHBF_enAU1047AU1047&amp;sxsrf=AM9HkKmR8dFtasrVNGZkMFIxGz5Wq06ZjA%3A1703525037148&amp;ei=rbqJZczSCOCWjuMPsMy_8AM&amp;oq=miranda+high+&amp;gs_lp=Egxnd3Mtd2l6LXNlcnAiDW1pcmFuZGEgaGlnaCAqAggAMg0QABiABBgUGIcCGMkDMgUQABiABDILEAAYgAQYigUYkgMyBRAAGIAEMgUQABiABDIKEAAYgAQYFBiHAjIFEAAYgAQyBRAAGIAEMgUQABiABDIFEAAYgARI7RNQ6AZY6AZwAXgAkAEAmAH0BqABuAyqAQM2LTK4AQHIAQD4AQHCAgoQABhHGNYEGLAD4gMEGAAgQYgGAZAGCA&amp;sclient=gws-wiz-serp&amp;lqi=ChNtaXJhbmRhIGhpZ2ggc2Nob29sSN-07OW4roCACForEAAQARACGAAYARgCIhNtaXJhbmRhIGhpZ2ggc2Nob29sKggIAhAAEAEQApIBBnNjaG9vbJoBI0NoWkRTVWhOTUc5blMwVkpRMEZuU1VOUGNqUnVSbVZuRUFFqgE7EAEyHhABIhpTQ3iPFiqMHHb-9vGb0lli1Rpc5Z8xE87GgDIXEAIiE21pcmFuZGEgaGlnaCBzY2hvb2w"/>
-    <hyperlink ref="D22" r:id="rId5"/>
-    <hyperlink ref="D25" r:id="rId6" display="mailto:official@younghorizonsschool.com"/>
-    <hyperlink ref="D26" r:id="rId7" display="mailto:iwanttojoin@siskol.edu.in"/>
-    <hyperlink ref="D27" r:id="rId8" display="mailto:lcgvm2012@gmail.com"/>
-    <hyperlink ref="D30" r:id="rId9"/>
-    <hyperlink ref="D33" r:id="rId10"/>
-    <hyperlink ref="D35" r:id="rId11"/>
-    <hyperlink ref="D37" r:id="rId12"/>
-    <hyperlink ref="D41" r:id="rId13"/>
-    <hyperlink ref="D42" r:id="rId14"/>
-    <hyperlink ref="D43" r:id="rId15"/>
-    <hyperlink ref="D47" r:id="rId16"/>
-    <hyperlink ref="D48" r:id="rId17"/>
-    <hyperlink ref="D49" r:id="rId18"/>
-    <hyperlink ref="D51" r:id="rId19"/>
-    <hyperlink ref="D52" r:id="rId20"/>
-    <hyperlink ref="D53" r:id="rId21"/>
-    <hyperlink ref="D54" r:id="rId22"/>
-    <hyperlink ref="D55" r:id="rId23"/>
-    <hyperlink ref="D56" r:id="rId24"/>
-    <hyperlink ref="D57" r:id="rId25"/>
-    <hyperlink ref="D58" r:id="rId26"/>
-    <hyperlink ref="D59" r:id="rId27"/>
-    <hyperlink ref="D60" r:id="rId28"/>
-    <hyperlink ref="D61" r:id="rId29"/>
-    <hyperlink ref="D62" r:id="rId30"/>
-    <hyperlink ref="D63" r:id="rId31"/>
-    <hyperlink ref="D64" r:id="rId32"/>
-    <hyperlink ref="D65" r:id="rId33"/>
-    <hyperlink ref="D66" r:id="rId34"/>
-    <hyperlink ref="D67" r:id="rId35"/>
-    <hyperlink ref="D68" r:id="rId36"/>
-    <hyperlink ref="D69" r:id="rId37"/>
-    <hyperlink ref="D70" r:id="rId38"/>
-    <hyperlink ref="D71" r:id="rId39"/>
-    <hyperlink ref="D72" r:id="rId40"/>
-    <hyperlink ref="D73" r:id="rId41"/>
-    <hyperlink ref="D75" r:id="rId42"/>
-    <hyperlink ref="D78" r:id="rId43"/>
-    <hyperlink ref="D79" r:id="rId44"/>
-    <hyperlink ref="D80" r:id="rId45"/>
-    <hyperlink ref="D81" r:id="rId46"/>
-    <hyperlink ref="D85" r:id="rId47"/>
-    <hyperlink ref="D88" r:id="rId48"/>
-    <hyperlink ref="D89" r:id="rId49"/>
-    <hyperlink ref="D91" r:id="rId50"/>
+    <hyperlink ref="D31" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D32" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E7" r:id="rId3" display="https://www.google.com/search?q=panchasayar+siksha+niketan&amp;sca_esv=593615924&amp;rlz=1C1CHBF_enAU1047AU1047&amp;sxsrf=AM9HkKnlKkWvrpmDIvMzNnJR8ZC_8s6gNQ%3A1703524925488&amp;ei=PbqJZaauHY2KnesPo--TuAo&amp;gs_ssp=eJzj4tFP1zc0MqnMzTa1TDNgtFI1qDBONDAyNzRPNU1LM0xOTkuyAgqZpJmZmJgnGZgZGSWnpSV5SRUk5iVnJBYnViYWKRRnZhdnJCrkZWanliTmAQC7Qxln&amp;oq=panchasayar+s&amp;gs_lp=Egxnd3Mtd2l6LXNlcnAiDXBhbmNoYXNheWFyIHMqAggAMhQQLhivARjHARimAxioAxiABBiOBTIFEAAYgAQyBRAAGIAEMgsQLhiABBioAxidAzIFEAAYgAQyBRAAGIAEMgUQABiABDIFEAAYgAQyCBAAGIAEGMsBMggQABiABBjLATIjEC4YrwEYxwEYpgMYqAMYgAQYjgUYlwUY3AQY3gQY4ATYAQNIuzhQmhhYmCVwAXgBkAEAmAGvAqAB1gSqAQUyLTEuMbgBAcgBAPgBAcICChAAGEcY1gQYsAPCAg0QABiABBiKBRhDGLADwgIcEC4YgAQYigUYQxjHARivARjIAxiwAxiOBdgBAcICGRAuGIAEGIoFGEMYxwEYrwEYyAMYsAPYAQHCAg4QABjkAhjWBBiwA9gBAsICEBAuGEMYnQMYqAMYgAQYigXCAhAQLhiABBiKBRhDGKgDGJ0DwgIWEC4YQxivARjHARimAxioAxiABBiKBcICChAAGIAEGBQYhwLCAh8QLhhDGJ0DGKgDGIAEGIoFGJcFGNwEGN4EGOAE2AED4gMEGAAgQYgGAZAGDroGBggBEAEYCLoGBggCEAEYCboGBggDEAEYFA&amp;sclient=gws-wiz-serp" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E8" r:id="rId4" display="https://www.google.com/search?q=miranda+high+school&amp;sca_esv=593615924&amp;rlz=1C1CHBF_enAU1047AU1047&amp;sxsrf=AM9HkKmR8dFtasrVNGZkMFIxGz5Wq06ZjA%3A1703525037148&amp;ei=rbqJZczSCOCWjuMPsMy_8AM&amp;oq=miranda+high+&amp;gs_lp=Egxnd3Mtd2l6LXNlcnAiDW1pcmFuZGEgaGlnaCAqAggAMg0QABiABBgUGIcCGMkDMgUQABiABDILEAAYgAQYigUYkgMyBRAAGIAEMgUQABiABDIKEAAYgAQYFBiHAjIFEAAYgAQyBRAAGIAEMgUQABiABDIFEAAYgARI7RNQ6AZY6AZwAXgAkAEAmAH0BqABuAyqAQM2LTK4AQHIAQD4AQHCAgoQABhHGNYEGLAD4gMEGAAgQYgGAZAGCA&amp;sclient=gws-wiz-serp&amp;lqi=ChNtaXJhbmRhIGhpZ2ggc2Nob29sSN-07OW4roCACForEAAQARACGAAYARgCIhNtaXJhbmRhIGhpZ2ggc2Nob29sKggIAhAAEAEQApIBBnNjaG9vbJoBI0NoWkRTVWhOTUc5blMwVkpRMEZuU1VOUGNqUnVSbVZuRUFFqgE7EAEyHhABIhpTQ3iPFiqMHHb-9vGb0lli1Rpc5Z8xE87GgDIXEAIiE21pcmFuZGEgaGlnaCBzY2hvb2w" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="D22" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="D25" r:id="rId6" display="mailto:official@younghorizonsschool.com" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="D26" r:id="rId7" display="mailto:iwanttojoin@siskol.edu.in" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="D27" r:id="rId8" display="mailto:lcgvm2012@gmail.com" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="D30" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="D33" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="D35" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="D37" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="D41" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="D42" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="D43" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="D47" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="D48" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="D49" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="D51" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="D52" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="D53" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="D54" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="D55" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="D56" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="D57" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="D58" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="D59" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="D60" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="D61" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="D62" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="D63" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="D64" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="D65" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="D66" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="D67" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="D68" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="D69" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="D70" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="D71" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="D72" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="D73" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="D75" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="D78" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="D79" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="D80" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="D81" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="D85" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="D88" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="D89" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="D91" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId51"/>
   <legacyDrawing r:id="rId52"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C62A7D6E-79B1-445C-8C29-27138C70C084}">
+  <dimension ref="A1:B122"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B122"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="31.2" x14ac:dyDescent="0.6"/>
+  <cols>
+    <col min="1" max="1" width="14.33203125" style="13" customWidth="1"/>
+    <col min="2" max="2" width="76.21875" style="13" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A2" s="15">
+        <v>1</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A3" s="15">
+        <v>2</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A4" s="15">
+        <v>3</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A5" s="15">
+        <v>4</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A6" s="15">
+        <v>5</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="29.4" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A7" s="15">
+        <v>6</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A8" s="15">
+        <v>7</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A9" s="15">
+        <v>8</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A10" s="15">
+        <v>9</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A11" s="15">
+        <v>10</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A12" s="15">
+        <v>11</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A13" s="15">
+        <v>12</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="39" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A14" s="15">
+        <v>13</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A15" s="15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A16" s="15">
+        <v>15</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A17" s="15">
+        <v>16</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A18" s="15">
+        <v>17</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A19" s="15">
+        <v>18</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="36.6" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A20" s="15">
+        <v>19</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A21" s="15">
+        <v>20</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A22" s="15">
+        <v>21</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A23" s="15">
+        <v>22</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A24" s="15">
+        <v>23</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A25" s="15">
+        <v>24</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A26" s="15">
+        <v>25</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A27" s="15">
+        <v>26</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A28" s="15">
+        <v>27</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A29" s="15">
+        <v>28</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A30" s="15">
+        <v>29</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A31" s="15">
+        <v>30</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A32" s="15">
+        <v>31</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A33" s="15">
+        <v>32</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A34" s="15">
+        <v>33</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A35" s="15">
+        <v>34</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A36" s="15">
+        <v>35</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A37" s="15">
+        <v>36</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A38" s="15">
+        <v>37</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A39" s="15">
+        <v>38</v>
+      </c>
+      <c r="B39" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A40" s="15">
+        <v>39</v>
+      </c>
+      <c r="B40" s="16" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A41" s="15">
+        <v>40</v>
+      </c>
+      <c r="B41" s="16" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A42" s="15">
+        <v>41</v>
+      </c>
+      <c r="B42" s="16" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A43" s="15">
+        <v>42</v>
+      </c>
+      <c r="B43" s="16" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A44" s="15">
+        <v>43</v>
+      </c>
+      <c r="B44" s="16" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A45" s="15">
+        <v>44</v>
+      </c>
+      <c r="B45" s="16" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A46" s="15">
+        <v>45</v>
+      </c>
+      <c r="B46" s="16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A47" s="15">
+        <v>46</v>
+      </c>
+      <c r="B47" s="16" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A48" s="15">
+        <v>47</v>
+      </c>
+      <c r="B48" s="16" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="33.6" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A49" s="15">
+        <v>48</v>
+      </c>
+      <c r="B49" s="16" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A50" s="15">
+        <v>49</v>
+      </c>
+      <c r="B50" s="16" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A51" s="15">
+        <v>50</v>
+      </c>
+      <c r="B51" s="16" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A52" s="15">
+        <v>51</v>
+      </c>
+      <c r="B52" s="16" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A53" s="15">
+        <v>52</v>
+      </c>
+      <c r="B53" s="16" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A54" s="15">
+        <v>53</v>
+      </c>
+      <c r="B54" s="16" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A55" s="15">
+        <v>54</v>
+      </c>
+      <c r="B55" s="16" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="33.6" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A56" s="15">
+        <v>55</v>
+      </c>
+      <c r="B56" s="16" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A57" s="15">
+        <v>56</v>
+      </c>
+      <c r="B57" s="16" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A58" s="15">
+        <v>57</v>
+      </c>
+      <c r="B58" s="16" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A59" s="15">
+        <v>58</v>
+      </c>
+      <c r="B59" s="16" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A60" s="15">
+        <v>59</v>
+      </c>
+      <c r="B60" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A61" s="15">
+        <v>60</v>
+      </c>
+      <c r="B61" s="16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A62" s="15">
+        <v>61</v>
+      </c>
+      <c r="B62" s="16" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A63" s="15">
+        <v>62</v>
+      </c>
+      <c r="B63" s="16" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A64" s="15">
+        <v>63</v>
+      </c>
+      <c r="B64" s="16" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A65" s="15">
+        <v>64</v>
+      </c>
+      <c r="B65" s="16" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A66" s="15">
+        <v>65</v>
+      </c>
+      <c r="B66" s="16" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A67" s="15">
+        <v>66</v>
+      </c>
+      <c r="B67" s="16" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A68" s="15">
+        <v>67</v>
+      </c>
+      <c r="B68" s="16" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A69" s="15">
+        <v>68</v>
+      </c>
+      <c r="B69" s="16" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A70" s="15">
+        <v>69</v>
+      </c>
+      <c r="B70" s="16" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A71" s="15">
+        <v>70</v>
+      </c>
+      <c r="B71" s="16" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A72" s="15">
+        <v>71</v>
+      </c>
+      <c r="B72" s="16" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A73" s="15">
+        <v>72</v>
+      </c>
+      <c r="B73" s="16" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A74" s="15">
+        <v>73</v>
+      </c>
+      <c r="B74" s="16" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A75" s="15">
+        <v>74</v>
+      </c>
+      <c r="B75" s="16" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A76" s="15">
+        <v>75</v>
+      </c>
+      <c r="B76" s="16" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A77" s="15">
+        <v>76</v>
+      </c>
+      <c r="B77" s="16" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A78" s="15">
+        <v>77</v>
+      </c>
+      <c r="B78" s="16" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A79" s="15">
+        <v>78</v>
+      </c>
+      <c r="B79" s="16" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A80" s="15">
+        <v>79</v>
+      </c>
+      <c r="B80" s="16" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A81" s="15">
+        <v>80</v>
+      </c>
+      <c r="B81" s="16" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A82" s="15">
+        <v>81</v>
+      </c>
+      <c r="B82" s="16" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A83" s="15">
+        <v>82</v>
+      </c>
+      <c r="B83" s="16" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A84" s="15">
+        <v>83</v>
+      </c>
+      <c r="B84" s="16" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A85" s="15">
+        <v>84</v>
+      </c>
+      <c r="B85" s="16" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="42.6" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A86" s="15">
+        <v>85</v>
+      </c>
+      <c r="B86" s="16" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A87" s="15">
+        <v>86</v>
+      </c>
+      <c r="B87" s="16" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A88" s="15">
+        <v>87</v>
+      </c>
+      <c r="B88" s="16" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A89" s="15">
+        <v>88</v>
+      </c>
+      <c r="B89" s="16" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A90" s="15">
+        <v>89</v>
+      </c>
+      <c r="B90" s="16" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A91" s="15">
+        <v>90</v>
+      </c>
+      <c r="B91" s="16" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A92" s="15">
+        <v>91</v>
+      </c>
+      <c r="B92" s="16" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A93" s="15">
+        <v>92</v>
+      </c>
+      <c r="B93" s="16" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A94" s="15">
+        <v>93</v>
+      </c>
+      <c r="B94" s="16" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A95" s="15">
+        <v>94</v>
+      </c>
+      <c r="B95" s="16" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A96" s="15">
+        <v>95</v>
+      </c>
+      <c r="B96" s="16" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A97" s="15">
+        <v>96</v>
+      </c>
+      <c r="B97" s="16" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A98" s="15">
+        <v>97</v>
+      </c>
+      <c r="B98" s="16" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A99" s="15">
+        <v>98</v>
+      </c>
+      <c r="B99" s="16" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A100" s="15">
+        <v>99</v>
+      </c>
+      <c r="B100" s="16" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A101" s="15">
+        <v>100</v>
+      </c>
+      <c r="B101" s="16" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A102" s="15">
+        <v>101</v>
+      </c>
+      <c r="B102" s="16" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A103" s="15">
+        <v>102</v>
+      </c>
+      <c r="B103" s="16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A104" s="15">
+        <v>103</v>
+      </c>
+      <c r="B104" s="16" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A105" s="15">
+        <v>104</v>
+      </c>
+      <c r="B105" s="16" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A106" s="15">
+        <v>105</v>
+      </c>
+      <c r="B106" s="16" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="51.6" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A107" s="15">
+        <v>106</v>
+      </c>
+      <c r="B107" s="16" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A108" s="15">
+        <v>107</v>
+      </c>
+      <c r="B108" s="16" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A109" s="15">
+        <v>108</v>
+      </c>
+      <c r="B109" s="16" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A110" s="15">
+        <v>109</v>
+      </c>
+      <c r="B110" s="16" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A111" s="15">
+        <v>110</v>
+      </c>
+      <c r="B111" s="16" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A112" s="15">
+        <v>111</v>
+      </c>
+      <c r="B112" s="16" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A113" s="15">
+        <v>112</v>
+      </c>
+      <c r="B113" s="16" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A114" s="15">
+        <v>113</v>
+      </c>
+      <c r="B114" s="16" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A115" s="15">
+        <v>114</v>
+      </c>
+      <c r="B115" s="16" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A116" s="15">
+        <v>115</v>
+      </c>
+      <c r="B116" s="16" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A117" s="15">
+        <v>116</v>
+      </c>
+      <c r="B117" s="16" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" ht="42.6" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A118" s="15">
+        <v>117</v>
+      </c>
+      <c r="B118" s="16" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A119" s="15">
+        <v>118</v>
+      </c>
+      <c r="B119" s="16" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A120" s="15">
+        <v>119</v>
+      </c>
+      <c r="B120" s="16" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A121" s="15">
+        <v>120</v>
+      </c>
+      <c r="B121" s="16" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A122" s="15">
+        <v>121</v>
+      </c>
+      <c r="B122" s="16" t="s">
+        <v>239</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update AI Workshop schools
Update AI Workshop schools
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Marketing/AI marketing/AI Workshop Schools.xlsx
+++ b/Offline/BusinessManagement/Marketing/AI marketing/AI Workshop Schools.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Marketing\AI marketing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F24E9D1-B47B-45EE-991D-4027E9678D5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F4ACB06-B6B8-45AA-9AE0-B4501389CB0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="280">
   <si>
     <t>CBSE</t>
   </si>
@@ -895,6 +895,27 @@
   </si>
   <si>
     <t>Achievement</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>Bad</t>
+  </si>
+  <si>
+    <t>School Rating</t>
+  </si>
+  <si>
+    <t>Total Good School</t>
+  </si>
+  <si>
+    <t>Total Bad School</t>
+  </si>
+  <si>
+    <t>Total Mediocre School</t>
+  </si>
+  <si>
+    <t>Mediocre</t>
   </si>
 </sst>
 </file>
@@ -990,7 +1011,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1013,12 +1034,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1069,9 +1116,13 @@
     <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1353,21 +1404,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DC48E2D-CE6A-43EF-B55A-B9B416B6A77B}">
-  <dimension ref="C2:K17"/>
+  <dimension ref="B2:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="21.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" customWidth="1"/>
-    <col min="11" max="11" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C2" s="16" t="s">
         <v>246</v>
       </c>
@@ -1375,8 +1429,13 @@
         <f>MAX('School-Details'!A:A)</f>
         <v>121</v>
       </c>
-    </row>
-    <row r="3" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="J2" s="14"/>
+      <c r="K2" s="24" t="s">
+        <v>211</v>
+      </c>
+      <c r="L2" s="25"/>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C3" s="16" t="s">
         <v>247</v>
       </c>
@@ -1384,59 +1443,76 @@
         <f>SUM('School-Details'!H:H)/D2</f>
         <v>0</v>
       </c>
-      <c r="I3" s="14"/>
-      <c r="J3" s="24" t="s">
-        <v>211</v>
-      </c>
-      <c r="K3" s="24"/>
-    </row>
-    <row r="4" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="I4" s="22" t="s">
+      <c r="J3" s="22" t="s">
         <v>270</v>
       </c>
-      <c r="J4" s="22" t="s">
+      <c r="K3" s="22" t="s">
         <v>271</v>
       </c>
-      <c r="K4" s="22" t="s">
+      <c r="L3" s="22" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="5" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="J4" s="23">
+        <v>45292</v>
+      </c>
+      <c r="K4" s="14">
+        <v>0</v>
+      </c>
+      <c r="L4" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C5" s="22" t="s">
         <v>248</v>
       </c>
       <c r="D5" s="22" t="s">
         <v>265</v>
       </c>
-      <c r="I5" s="23">
-        <v>45292</v>
-      </c>
-      <c r="J5" s="14">
-        <v>0</v>
+      <c r="F5" s="22" t="s">
+        <v>266</v>
+      </c>
+      <c r="G5" s="22" t="s">
+        <v>267</v>
+      </c>
+      <c r="J5" s="23">
+        <v>45323</v>
       </c>
       <c r="K5" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="L5" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C6" s="14" t="s">
         <v>252</v>
       </c>
       <c r="D6" s="14">
         <f>COUNTIF('School-Details'!R:R,C6)</f>
-        <v>2</v>
-      </c>
-      <c r="I6" s="23">
-        <v>45323</v>
-      </c>
-      <c r="J6" s="14">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="G6" s="14">
+        <f>COUNTIF('School-Details'!J:J,F6)</f>
+        <v>0</v>
+      </c>
+      <c r="J6" s="23">
+        <v>45352</v>
       </c>
       <c r="K6" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="L6" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C7" s="14" t="s">
         <v>254</v>
       </c>
@@ -1444,17 +1520,24 @@
         <f>COUNTIF('School-Details'!R:R,C7)</f>
         <v>0</v>
       </c>
-      <c r="I7" s="23">
-        <v>45352</v>
-      </c>
-      <c r="J7" s="14">
-        <v>0</v>
+      <c r="F7" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="G7" s="14">
+        <f>COUNTIF('School-Details'!J:J,F7)</f>
+        <v>0</v>
+      </c>
+      <c r="J7" s="23">
+        <v>45383</v>
       </c>
       <c r="K7" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="L7" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C8" s="14" t="s">
         <v>256</v>
       </c>
@@ -1462,17 +1545,24 @@
         <f>COUNTIF('School-Details'!R:R,C8)</f>
         <v>0</v>
       </c>
-      <c r="I8" s="23">
-        <v>45383</v>
-      </c>
-      <c r="J8" s="14">
-        <v>0</v>
+      <c r="F8" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="G8" s="14">
+        <f>COUNTIF('School-Details'!J:J,F8)</f>
+        <v>0</v>
+      </c>
+      <c r="J8" s="23">
+        <v>45413</v>
       </c>
       <c r="K8" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="L8" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C9" s="14" t="s">
         <v>258</v>
       </c>
@@ -1480,17 +1570,17 @@
         <f>COUNTIF('School-Details'!R:R,C9)</f>
         <v>0</v>
       </c>
-      <c r="I9" s="23">
-        <v>45413</v>
-      </c>
-      <c r="J9" s="14">
-        <v>0</v>
+      <c r="J9" s="23">
+        <v>45444</v>
       </c>
       <c r="K9" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="L9" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C10" s="14" t="s">
         <v>260</v>
       </c>
@@ -1498,17 +1588,17 @@
         <f>COUNTIF('School-Details'!R:R,C10)</f>
         <v>0</v>
       </c>
-      <c r="I10" s="23">
-        <v>45444</v>
-      </c>
-      <c r="J10" s="14">
-        <v>0</v>
+      <c r="J10" s="23">
+        <v>45474</v>
       </c>
       <c r="K10" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="L10" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C11" s="14" t="s">
         <v>262</v>
       </c>
@@ -1516,121 +1606,172 @@
         <f>COUNTIF('School-Details'!R:R,C11)</f>
         <v>0</v>
       </c>
-      <c r="I11" s="23">
-        <v>45474</v>
-      </c>
-      <c r="J11" s="14">
-        <v>0</v>
+      <c r="J11" s="23">
+        <v>45505</v>
       </c>
       <c r="K11" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="L11" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C12" s="14" t="s">
         <v>264</v>
       </c>
       <c r="D12" s="14">
         <f>COUNTIF('School-Details'!R:R,C12)</f>
-        <v>119</v>
-      </c>
-      <c r="I12" s="23">
-        <v>45505</v>
-      </c>
-      <c r="J12" s="14">
-        <v>0</v>
+        <v>121</v>
+      </c>
+      <c r="J12" s="23">
+        <v>45536</v>
       </c>
       <c r="K12" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="I13" s="23">
-        <v>45536</v>
-      </c>
-      <c r="J13" s="14">
-        <v>0</v>
+      <c r="L12" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="J13" s="23">
+        <v>45566</v>
       </c>
       <c r="K13" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="L13" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B14" s="26"/>
       <c r="C14" s="22" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>267</v>
-      </c>
-      <c r="I14" s="23">
-        <v>45566</v>
-      </c>
-      <c r="J14" s="14">
-        <v>0</v>
+        <v>265</v>
+      </c>
+      <c r="J14" s="23">
+        <v>45597</v>
       </c>
       <c r="K14" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C15" s="14" t="s">
-        <v>211</v>
+      <c r="L14" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B15" s="14" t="s">
+        <v>273</v>
+      </c>
+      <c r="C15" s="14">
+        <v>5</v>
       </c>
       <c r="D15" s="14">
-        <f>COUNTIF('School-Details'!J:J,C15)</f>
+        <f>COUNTIF('School-Details'!Q:Q,C15)</f>
+        <v>8</v>
+      </c>
+      <c r="J15" s="23">
+        <v>45627</v>
+      </c>
+      <c r="K15" s="14">
+        <v>0</v>
+      </c>
+      <c r="L15" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B16" s="14"/>
+      <c r="C16" s="14">
+        <v>4</v>
+      </c>
+      <c r="D16" s="14">
+        <f>COUNTIF('School-Details'!Q:Q,C16)</f>
+        <v>35</v>
+      </c>
+      <c r="J16" s="16" t="s">
+        <v>245</v>
+      </c>
+      <c r="K16" s="16">
+        <f>SUM(K4:K15)</f>
+        <v>0</v>
+      </c>
+      <c r="L16" s="16">
+        <f>SUM(L4:L15)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B17" s="14"/>
+      <c r="C17" s="14" t="s">
+        <v>276</v>
+      </c>
+      <c r="D17" s="14">
+        <f>SUM(D15:D16)</f>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B18" s="14" t="s">
+        <v>279</v>
+      </c>
+      <c r="C18" s="14">
+        <v>3</v>
+      </c>
+      <c r="D18" s="14">
+        <f>COUNTIF('School-Details'!Q:Q,C18)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B19" s="14"/>
+      <c r="C19" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="D19" s="14">
+        <f>SUM(D18)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B20" s="14" t="s">
+        <v>274</v>
+      </c>
+      <c r="C20" s="14">
         <v>2</v>
       </c>
-      <c r="I15" s="23">
-        <v>45597</v>
-      </c>
-      <c r="J15" s="14">
-        <v>0</v>
-      </c>
-      <c r="K15" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C16" s="14" t="s">
-        <v>268</v>
-      </c>
-      <c r="D16" s="14">
-        <f>COUNTIF('School-Details'!J:J,C16)</f>
-        <v>0</v>
-      </c>
-      <c r="I16" s="23">
-        <v>45627</v>
-      </c>
-      <c r="J16" s="14">
-        <v>0</v>
-      </c>
-      <c r="K16" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C17" s="14" t="s">
-        <v>269</v>
-      </c>
-      <c r="D17" s="14">
-        <f>COUNTIF('School-Details'!J:J,C17)</f>
-        <v>0</v>
-      </c>
-      <c r="I17" s="16" t="s">
-        <v>245</v>
-      </c>
-      <c r="J17" s="16">
-        <f>SUM(J5:J16)</f>
-        <v>0</v>
-      </c>
-      <c r="K17" s="16">
-        <f>SUM(K5:K16)</f>
-        <v>0</v>
+      <c r="D20" s="14">
+        <f>COUNTIF('School-Details'!Q:Q,C20)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B21" s="14"/>
+      <c r="C21" s="14">
+        <v>1</v>
+      </c>
+      <c r="D21" s="14">
+        <f>COUNTIF('School-Details'!Q:Q,C21)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B22" s="14"/>
+      <c r="C22" s="14" t="s">
+        <v>277</v>
+      </c>
+      <c r="D22" s="14">
+        <f>SUM(D20:D21)</f>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="K2:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1641,12 +1782,15 @@
   <dimension ref="A1:R122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <pane xSplit="5" ySplit="6" topLeftCell="I7" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="K123" sqref="K123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="25.6640625" style="17" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="46.5546875" style="1" bestFit="1" customWidth="1"/>
@@ -1731,13 +1875,29 @@
       <c r="E2" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
+      <c r="K2" s="10">
+        <v>5</v>
+      </c>
+      <c r="L2" s="10">
+        <v>3</v>
+      </c>
+      <c r="M2" s="10">
+        <v>4</v>
+      </c>
+      <c r="N2" s="10">
+        <v>5</v>
+      </c>
+      <c r="O2" s="10">
+        <v>3</v>
+      </c>
+      <c r="P2" s="10">
+        <f>SUM(K2:O2)</f>
+        <v>20</v>
+      </c>
+      <c r="Q2" s="10">
+        <f>ROUND(P2/5,0)</f>
+        <v>4</v>
+      </c>
       <c r="R2" s="10" t="s">
         <v>264</v>
       </c>
@@ -1752,13 +1912,29 @@
       <c r="E3" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
+      <c r="K3" s="10">
+        <v>5</v>
+      </c>
+      <c r="L3" s="10">
+        <v>3</v>
+      </c>
+      <c r="M3" s="10">
+        <v>3</v>
+      </c>
+      <c r="N3" s="10">
+        <v>3</v>
+      </c>
+      <c r="O3" s="10">
+        <v>2</v>
+      </c>
+      <c r="P3" s="10">
+        <f t="shared" ref="P3:P66" si="0">SUM(K3:O3)</f>
+        <v>16</v>
+      </c>
+      <c r="Q3" s="10">
+        <f>ROUND(P3/5,0)</f>
+        <v>3</v>
+      </c>
       <c r="R3" s="10" t="s">
         <v>264</v>
       </c>
@@ -1779,11 +1955,31 @@
       <c r="F4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>211</v>
+      <c r="K4" s="10">
+        <v>5</v>
+      </c>
+      <c r="L4" s="10">
+        <v>3</v>
+      </c>
+      <c r="M4" s="10">
+        <v>2</v>
+      </c>
+      <c r="N4" s="10">
+        <v>2</v>
+      </c>
+      <c r="O4" s="10">
+        <v>2</v>
+      </c>
+      <c r="P4" s="10">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="Q4" s="10">
+        <f t="shared" ref="Q4:Q67" si="1">ROUND(P4/5,0)</f>
+        <v>3</v>
       </c>
       <c r="R4" s="10" t="s">
-        <v>252</v>
+        <v>264</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
@@ -1796,11 +1992,34 @@
       <c r="E5" s="7" t="s">
         <v>45</v>
       </c>
+      <c r="K5" s="10">
+        <v>5</v>
+      </c>
+      <c r="L5" s="10">
+        <v>3</v>
+      </c>
+      <c r="M5" s="10">
+        <v>4</v>
+      </c>
+      <c r="N5" s="10">
+        <v>4</v>
+      </c>
+      <c r="O5" s="10">
+        <v>3</v>
+      </c>
+      <c r="P5" s="10">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="Q5" s="10">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
       <c r="R5" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1809,6 +2028,29 @@
       </c>
       <c r="E6" s="8" t="s">
         <v>46</v>
+      </c>
+      <c r="K6" s="10">
+        <v>5</v>
+      </c>
+      <c r="L6" s="10">
+        <v>3</v>
+      </c>
+      <c r="M6" s="10">
+        <v>3</v>
+      </c>
+      <c r="N6" s="10">
+        <v>3</v>
+      </c>
+      <c r="O6" s="10">
+        <v>2</v>
+      </c>
+      <c r="P6" s="10">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="Q6" s="10">
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
       <c r="R6" s="10" t="s">
         <v>264</v>
@@ -1824,6 +2066,29 @@
       <c r="E7" s="9" t="s">
         <v>47</v>
       </c>
+      <c r="K7" s="10">
+        <v>5</v>
+      </c>
+      <c r="L7" s="10">
+        <v>3</v>
+      </c>
+      <c r="M7" s="10">
+        <v>3</v>
+      </c>
+      <c r="N7" s="10">
+        <v>3</v>
+      </c>
+      <c r="O7" s="10">
+        <v>4</v>
+      </c>
+      <c r="P7" s="10">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="Q7" s="10">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
       <c r="R7" s="10" t="s">
         <v>264</v>
       </c>
@@ -1838,6 +2103,29 @@
       <c r="E8" s="9" t="s">
         <v>48</v>
       </c>
+      <c r="K8" s="10">
+        <v>5</v>
+      </c>
+      <c r="L8" s="10">
+        <v>2</v>
+      </c>
+      <c r="M8" s="10">
+        <v>2</v>
+      </c>
+      <c r="N8" s="10">
+        <v>3</v>
+      </c>
+      <c r="O8" s="10">
+        <v>2</v>
+      </c>
+      <c r="P8" s="10">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="Q8" s="10">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
       <c r="R8" s="10" t="s">
         <v>264</v>
       </c>
@@ -1855,6 +2143,29 @@
       <c r="E9" s="7" t="s">
         <v>50</v>
       </c>
+      <c r="K9" s="10">
+        <v>4</v>
+      </c>
+      <c r="L9" s="10">
+        <v>4</v>
+      </c>
+      <c r="M9" s="10">
+        <v>5</v>
+      </c>
+      <c r="N9" s="10">
+        <v>5</v>
+      </c>
+      <c r="O9" s="10">
+        <v>3</v>
+      </c>
+      <c r="P9" s="10">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="Q9" s="10">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
       <c r="R9" s="10" t="s">
         <v>264</v>
       </c>
@@ -1869,6 +2180,29 @@
       <c r="E10" s="7">
         <v>9051770999</v>
       </c>
+      <c r="K10" s="10">
+        <v>3</v>
+      </c>
+      <c r="L10" s="10">
+        <v>4</v>
+      </c>
+      <c r="M10" s="10">
+        <v>5</v>
+      </c>
+      <c r="N10" s="10">
+        <v>5</v>
+      </c>
+      <c r="O10" s="10">
+        <v>5</v>
+      </c>
+      <c r="P10" s="10">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="Q10" s="10">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
       <c r="R10" s="10" t="s">
         <v>264</v>
       </c>
@@ -1883,6 +2217,29 @@
       <c r="E11" s="7">
         <v>9903606575</v>
       </c>
+      <c r="K11" s="10">
+        <v>4</v>
+      </c>
+      <c r="L11" s="10">
+        <v>5</v>
+      </c>
+      <c r="M11" s="10">
+        <v>4</v>
+      </c>
+      <c r="N11" s="10">
+        <v>4</v>
+      </c>
+      <c r="O11" s="10">
+        <v>4</v>
+      </c>
+      <c r="P11" s="10">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="Q11" s="10">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
       <c r="R11" s="10" t="s">
         <v>264</v>
       </c>
@@ -1897,6 +2254,29 @@
       <c r="E12" s="7" t="s">
         <v>51</v>
       </c>
+      <c r="K12" s="10">
+        <v>4</v>
+      </c>
+      <c r="L12" s="10">
+        <v>5</v>
+      </c>
+      <c r="M12" s="10">
+        <v>5</v>
+      </c>
+      <c r="N12" s="10">
+        <v>5</v>
+      </c>
+      <c r="O12" s="10">
+        <v>4</v>
+      </c>
+      <c r="P12" s="10">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="Q12" s="10">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
       <c r="R12" s="10" t="s">
         <v>264</v>
       </c>
@@ -1911,6 +2291,29 @@
       <c r="E13" s="7" t="s">
         <v>52</v>
       </c>
+      <c r="K13" s="10">
+        <v>4</v>
+      </c>
+      <c r="L13" s="10">
+        <v>5</v>
+      </c>
+      <c r="M13" s="10">
+        <v>5</v>
+      </c>
+      <c r="N13" s="10">
+        <v>5</v>
+      </c>
+      <c r="O13" s="10">
+        <v>4</v>
+      </c>
+      <c r="P13" s="10">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="Q13" s="10">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
       <c r="R13" s="10" t="s">
         <v>264</v>
       </c>
@@ -1925,6 +2328,29 @@
       <c r="E14" s="7" t="s">
         <v>56</v>
       </c>
+      <c r="K14" s="10">
+        <v>3</v>
+      </c>
+      <c r="L14" s="10">
+        <v>5</v>
+      </c>
+      <c r="M14" s="10">
+        <v>5</v>
+      </c>
+      <c r="N14" s="10">
+        <v>4</v>
+      </c>
+      <c r="O14" s="10">
+        <v>3</v>
+      </c>
+      <c r="P14" s="10">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="Q14" s="10">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
       <c r="R14" s="10" t="s">
         <v>264</v>
       </c>
@@ -1939,6 +2365,29 @@
       <c r="E15" s="7" t="s">
         <v>54</v>
       </c>
+      <c r="K15" s="10">
+        <v>3</v>
+      </c>
+      <c r="L15" s="10">
+        <v>5</v>
+      </c>
+      <c r="M15" s="10">
+        <v>5</v>
+      </c>
+      <c r="N15" s="10">
+        <v>5</v>
+      </c>
+      <c r="O15" s="10">
+        <v>4</v>
+      </c>
+      <c r="P15" s="10">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="Q15" s="10">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
       <c r="R15" s="10" t="s">
         <v>264</v>
       </c>
@@ -1953,6 +2402,29 @@
       <c r="E16" s="7" t="s">
         <v>57</v>
       </c>
+      <c r="K16" s="10">
+        <v>4</v>
+      </c>
+      <c r="L16" s="10">
+        <v>5</v>
+      </c>
+      <c r="M16" s="10">
+        <v>5</v>
+      </c>
+      <c r="N16" s="10">
+        <v>5</v>
+      </c>
+      <c r="O16" s="10">
+        <v>5</v>
+      </c>
+      <c r="P16" s="10">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="Q16" s="10">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
       <c r="R16" s="10" t="s">
         <v>264</v>
       </c>
@@ -1967,6 +2439,29 @@
       <c r="E17" s="7" t="s">
         <v>58</v>
       </c>
+      <c r="K17" s="10">
+        <v>3</v>
+      </c>
+      <c r="L17" s="10">
+        <v>4</v>
+      </c>
+      <c r="M17" s="10">
+        <v>3</v>
+      </c>
+      <c r="N17" s="10">
+        <v>4</v>
+      </c>
+      <c r="O17" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="P17" s="10">
+        <f t="shared" si="0"/>
+        <v>17.5</v>
+      </c>
+      <c r="Q17" s="10">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
       <c r="R17" s="10" t="s">
         <v>264</v>
       </c>
@@ -1981,6 +2476,29 @@
       <c r="E18" s="7" t="s">
         <v>59</v>
       </c>
+      <c r="K18" s="10">
+        <v>4</v>
+      </c>
+      <c r="L18" s="10">
+        <v>5</v>
+      </c>
+      <c r="M18" s="10">
+        <v>5</v>
+      </c>
+      <c r="N18" s="10">
+        <v>4</v>
+      </c>
+      <c r="O18" s="10">
+        <v>5</v>
+      </c>
+      <c r="P18" s="10">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="Q18" s="10">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
       <c r="R18" s="10" t="s">
         <v>264</v>
       </c>
@@ -1995,6 +2513,29 @@
       <c r="E19" s="7" t="s">
         <v>60</v>
       </c>
+      <c r="K19" s="10">
+        <v>4</v>
+      </c>
+      <c r="L19" s="10">
+        <v>3</v>
+      </c>
+      <c r="M19" s="10">
+        <v>3</v>
+      </c>
+      <c r="N19" s="10">
+        <v>4</v>
+      </c>
+      <c r="O19" s="10">
+        <v>2.5</v>
+      </c>
+      <c r="P19" s="10">
+        <f t="shared" si="0"/>
+        <v>16.5</v>
+      </c>
+      <c r="Q19" s="10">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
       <c r="R19" s="10" t="s">
         <v>264</v>
       </c>
@@ -2012,6 +2553,29 @@
       <c r="E20" s="7" t="s">
         <v>61</v>
       </c>
+      <c r="K20" s="10">
+        <v>4</v>
+      </c>
+      <c r="L20" s="10">
+        <v>4</v>
+      </c>
+      <c r="M20" s="10">
+        <v>3</v>
+      </c>
+      <c r="N20" s="10">
+        <v>3</v>
+      </c>
+      <c r="O20" s="10">
+        <v>3</v>
+      </c>
+      <c r="P20" s="10">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="Q20" s="10">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
       <c r="R20" s="10" t="s">
         <v>264</v>
       </c>
@@ -2029,6 +2593,29 @@
       <c r="E21" s="7" t="s">
         <v>61</v>
       </c>
+      <c r="K21" s="10">
+        <v>3</v>
+      </c>
+      <c r="L21" s="10">
+        <v>4</v>
+      </c>
+      <c r="M21" s="10">
+        <v>3</v>
+      </c>
+      <c r="N21" s="10">
+        <v>3</v>
+      </c>
+      <c r="O21" s="10">
+        <v>2.5</v>
+      </c>
+      <c r="P21" s="10">
+        <f t="shared" si="0"/>
+        <v>15.5</v>
+      </c>
+      <c r="Q21" s="10">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
       <c r="R21" s="10" t="s">
         <v>264</v>
       </c>
@@ -2046,6 +2633,29 @@
       <c r="E22" s="7">
         <v>8240520804</v>
       </c>
+      <c r="K22" s="10">
+        <v>3</v>
+      </c>
+      <c r="L22" s="10">
+        <v>4</v>
+      </c>
+      <c r="M22" s="10">
+        <v>5</v>
+      </c>
+      <c r="N22" s="10">
+        <v>5</v>
+      </c>
+      <c r="O22" s="10">
+        <v>4.5</v>
+      </c>
+      <c r="P22" s="10">
+        <f t="shared" si="0"/>
+        <v>21.5</v>
+      </c>
+      <c r="Q22" s="10">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
       <c r="R22" s="10" t="s">
         <v>264</v>
       </c>
@@ -2063,6 +2673,29 @@
       <c r="E23" s="7" t="s">
         <v>62</v>
       </c>
+      <c r="K23" s="10">
+        <v>4</v>
+      </c>
+      <c r="L23" s="10">
+        <v>4</v>
+      </c>
+      <c r="M23" s="10">
+        <v>4</v>
+      </c>
+      <c r="N23" s="10">
+        <v>3</v>
+      </c>
+      <c r="O23" s="10">
+        <v>2.5</v>
+      </c>
+      <c r="P23" s="10">
+        <f t="shared" si="0"/>
+        <v>17.5</v>
+      </c>
+      <c r="Q23" s="10">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
       <c r="R23" s="10" t="s">
         <v>264</v>
       </c>
@@ -2080,6 +2713,29 @@
       <c r="E24" s="7">
         <v>8961111167</v>
       </c>
+      <c r="K24" s="10">
+        <v>3</v>
+      </c>
+      <c r="L24" s="10">
+        <v>5</v>
+      </c>
+      <c r="M24" s="10">
+        <v>5</v>
+      </c>
+      <c r="N24" s="10">
+        <v>4</v>
+      </c>
+      <c r="O24" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="P24" s="10">
+        <f t="shared" si="0"/>
+        <v>20.5</v>
+      </c>
+      <c r="Q24" s="10">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
       <c r="R24" s="10" t="s">
         <v>264</v>
       </c>
@@ -2097,6 +2753,29 @@
       <c r="E25" s="7" t="s">
         <v>67</v>
       </c>
+      <c r="K25" s="10">
+        <v>4</v>
+      </c>
+      <c r="L25" s="10">
+        <v>3</v>
+      </c>
+      <c r="M25" s="10">
+        <v>4</v>
+      </c>
+      <c r="N25" s="10">
+        <v>4</v>
+      </c>
+      <c r="O25" s="10">
+        <v>2.5</v>
+      </c>
+      <c r="P25" s="10">
+        <f t="shared" si="0"/>
+        <v>17.5</v>
+      </c>
+      <c r="Q25" s="10">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
       <c r="R25" s="10" t="s">
         <v>264</v>
       </c>
@@ -2114,6 +2793,29 @@
       <c r="E26" s="7" t="s">
         <v>69</v>
       </c>
+      <c r="K26" s="10">
+        <v>3</v>
+      </c>
+      <c r="L26" s="10">
+        <v>5</v>
+      </c>
+      <c r="M26" s="10">
+        <v>5</v>
+      </c>
+      <c r="N26" s="10">
+        <v>5</v>
+      </c>
+      <c r="O26" s="10">
+        <v>4</v>
+      </c>
+      <c r="P26" s="10">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="Q26" s="10">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
       <c r="R26" s="10" t="s">
         <v>264</v>
       </c>
@@ -2131,6 +2833,29 @@
       <c r="E27" s="7">
         <v>7044096127</v>
       </c>
+      <c r="K27" s="10">
+        <v>3</v>
+      </c>
+      <c r="L27" s="10">
+        <v>4</v>
+      </c>
+      <c r="M27" s="10">
+        <v>4</v>
+      </c>
+      <c r="N27" s="10">
+        <v>4</v>
+      </c>
+      <c r="O27" s="10">
+        <v>4</v>
+      </c>
+      <c r="P27" s="10">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="Q27" s="10">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
       <c r="R27" s="10" t="s">
         <v>264</v>
       </c>
@@ -2145,6 +2870,29 @@
       <c r="E28" s="7" t="s">
         <v>72</v>
       </c>
+      <c r="K28" s="10">
+        <v>3</v>
+      </c>
+      <c r="L28" s="10">
+        <v>3</v>
+      </c>
+      <c r="M28" s="10">
+        <v>3</v>
+      </c>
+      <c r="N28" s="10">
+        <v>3</v>
+      </c>
+      <c r="O28" s="10">
+        <v>2.5</v>
+      </c>
+      <c r="P28" s="10">
+        <f t="shared" si="0"/>
+        <v>14.5</v>
+      </c>
+      <c r="Q28" s="10">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
       <c r="R28" s="10" t="s">
         <v>264</v>
       </c>
@@ -2159,6 +2907,29 @@
       <c r="E29" s="7">
         <v>9831274629</v>
       </c>
+      <c r="K29" s="10">
+        <v>4</v>
+      </c>
+      <c r="L29" s="10">
+        <v>3</v>
+      </c>
+      <c r="M29" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="N29" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="O29" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="P29" s="10">
+        <f t="shared" si="0"/>
+        <v>17.5</v>
+      </c>
+      <c r="Q29" s="10">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
       <c r="R29" s="10" t="s">
         <v>264</v>
       </c>
@@ -2176,6 +2947,29 @@
       <c r="E30" s="7">
         <v>8777257554</v>
       </c>
+      <c r="K30" s="10">
+        <v>4</v>
+      </c>
+      <c r="L30" s="10">
+        <v>3</v>
+      </c>
+      <c r="M30" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="N30" s="10">
+        <v>2.5</v>
+      </c>
+      <c r="O30" s="10">
+        <v>2.5</v>
+      </c>
+      <c r="P30" s="10">
+        <f t="shared" si="0"/>
+        <v>15.5</v>
+      </c>
+      <c r="Q30" s="10">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
       <c r="R30" s="10" t="s">
         <v>264</v>
       </c>
@@ -2193,6 +2987,29 @@
       <c r="E31" s="7" t="s">
         <v>75</v>
       </c>
+      <c r="K31" s="10">
+        <v>2.5</v>
+      </c>
+      <c r="L31" s="10">
+        <v>4.5</v>
+      </c>
+      <c r="M31" s="10">
+        <v>4.5</v>
+      </c>
+      <c r="N31" s="10">
+        <v>4</v>
+      </c>
+      <c r="O31" s="10">
+        <v>3</v>
+      </c>
+      <c r="P31" s="10">
+        <f t="shared" si="0"/>
+        <v>18.5</v>
+      </c>
+      <c r="Q31" s="10">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
       <c r="R31" s="10" t="s">
         <v>264</v>
       </c>
@@ -2210,6 +3027,29 @@
       <c r="E32" s="7" t="s">
         <v>76</v>
       </c>
+      <c r="K32" s="10">
+        <v>3</v>
+      </c>
+      <c r="L32" s="10">
+        <v>5</v>
+      </c>
+      <c r="M32" s="10">
+        <v>5</v>
+      </c>
+      <c r="N32" s="10">
+        <v>5</v>
+      </c>
+      <c r="O32" s="10">
+        <v>4</v>
+      </c>
+      <c r="P32" s="10">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="Q32" s="10">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
       <c r="R32" s="10" t="s">
         <v>264</v>
       </c>
@@ -2230,6 +3070,29 @@
       <c r="E33" s="7">
         <v>3322651531</v>
       </c>
+      <c r="K33" s="10">
+        <v>2</v>
+      </c>
+      <c r="L33" s="10">
+        <v>4</v>
+      </c>
+      <c r="M33" s="10">
+        <v>4</v>
+      </c>
+      <c r="N33" s="10">
+        <v>4</v>
+      </c>
+      <c r="O33" s="10">
+        <v>3</v>
+      </c>
+      <c r="P33" s="10">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="Q33" s="10">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
       <c r="R33" s="10" t="s">
         <v>264</v>
       </c>
@@ -2247,6 +3110,29 @@
       <c r="E34" s="7">
         <v>3324753015</v>
       </c>
+      <c r="K34" s="10">
+        <v>3</v>
+      </c>
+      <c r="L34" s="10">
+        <v>3</v>
+      </c>
+      <c r="M34" s="10">
+        <v>5</v>
+      </c>
+      <c r="N34" s="10">
+        <v>4</v>
+      </c>
+      <c r="O34" s="10">
+        <v>3</v>
+      </c>
+      <c r="P34" s="10">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="Q34" s="10">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
       <c r="R34" s="10" t="s">
         <v>264</v>
       </c>
@@ -2267,6 +3153,29 @@
       <c r="E35" s="7">
         <v>3340196666</v>
       </c>
+      <c r="K35" s="10">
+        <v>3</v>
+      </c>
+      <c r="L35" s="10">
+        <v>4</v>
+      </c>
+      <c r="M35" s="10">
+        <v>5</v>
+      </c>
+      <c r="N35" s="10">
+        <v>5</v>
+      </c>
+      <c r="O35" s="10">
+        <v>4</v>
+      </c>
+      <c r="P35" s="10">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="Q35" s="10">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
       <c r="R35" s="10" t="s">
         <v>264</v>
       </c>
@@ -2287,6 +3196,29 @@
       <c r="E36" s="7">
         <v>3324753765</v>
       </c>
+      <c r="K36" s="10">
+        <v>3</v>
+      </c>
+      <c r="L36" s="10">
+        <v>3</v>
+      </c>
+      <c r="M36" s="10">
+        <v>3</v>
+      </c>
+      <c r="N36" s="10">
+        <v>5</v>
+      </c>
+      <c r="O36" s="10">
+        <v>2</v>
+      </c>
+      <c r="P36" s="10">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="Q36" s="10">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
       <c r="R36" s="10" t="s">
         <v>264</v>
       </c>
@@ -2307,6 +3239,29 @@
       <c r="E37" s="7">
         <v>3324286903</v>
       </c>
+      <c r="K37" s="10">
+        <v>4</v>
+      </c>
+      <c r="L37" s="10">
+        <v>3</v>
+      </c>
+      <c r="M37" s="10">
+        <v>3</v>
+      </c>
+      <c r="N37" s="10">
+        <v>4</v>
+      </c>
+      <c r="O37" s="10">
+        <v>4</v>
+      </c>
+      <c r="P37" s="10">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="Q37" s="10">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
       <c r="R37" s="10" t="s">
         <v>264</v>
       </c>
@@ -2324,6 +3279,29 @@
       <c r="E38" s="8">
         <v>8902488077</v>
       </c>
+      <c r="K38" s="10">
+        <v>2</v>
+      </c>
+      <c r="L38" s="10">
+        <v>4</v>
+      </c>
+      <c r="M38" s="10">
+        <v>4</v>
+      </c>
+      <c r="N38" s="10">
+        <v>5</v>
+      </c>
+      <c r="O38" s="10">
+        <v>3</v>
+      </c>
+      <c r="P38" s="10">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="Q38" s="10">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
       <c r="R38" s="10" t="s">
         <v>264</v>
       </c>
@@ -2338,6 +3316,29 @@
       <c r="E39" s="9">
         <v>9163741069</v>
       </c>
+      <c r="K39" s="10">
+        <v>3</v>
+      </c>
+      <c r="L39" s="10">
+        <v>4</v>
+      </c>
+      <c r="M39" s="10">
+        <v>4</v>
+      </c>
+      <c r="N39" s="10">
+        <v>4</v>
+      </c>
+      <c r="O39" s="10">
+        <v>3</v>
+      </c>
+      <c r="P39" s="10">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="Q39" s="10">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
       <c r="R39" s="10" t="s">
         <v>264</v>
       </c>
@@ -2355,6 +3356,29 @@
       <c r="E40" s="9">
         <v>3324411691</v>
       </c>
+      <c r="K40" s="10">
+        <v>2</v>
+      </c>
+      <c r="L40" s="10">
+        <v>3</v>
+      </c>
+      <c r="M40" s="10">
+        <v>3</v>
+      </c>
+      <c r="N40" s="10">
+        <v>3</v>
+      </c>
+      <c r="O40" s="10">
+        <v>3</v>
+      </c>
+      <c r="P40" s="10">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="Q40" s="10">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
       <c r="R40" s="10" t="s">
         <v>264</v>
       </c>
@@ -2375,6 +3399,29 @@
       <c r="E41" s="7">
         <v>3324413804</v>
       </c>
+      <c r="K41" s="10">
+        <v>4</v>
+      </c>
+      <c r="L41" s="10">
+        <v>4</v>
+      </c>
+      <c r="M41" s="10">
+        <v>5</v>
+      </c>
+      <c r="N41" s="10">
+        <v>5</v>
+      </c>
+      <c r="O41" s="10">
+        <v>3</v>
+      </c>
+      <c r="P41" s="10">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="Q41" s="10">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
       <c r="R41" s="10" t="s">
         <v>264</v>
       </c>
@@ -2395,6 +3442,29 @@
       <c r="E42" s="7">
         <v>9830688888</v>
       </c>
+      <c r="K42" s="10">
+        <v>2</v>
+      </c>
+      <c r="L42" s="10">
+        <v>5</v>
+      </c>
+      <c r="M42" s="10">
+        <v>5</v>
+      </c>
+      <c r="N42" s="10">
+        <v>5</v>
+      </c>
+      <c r="O42" s="10">
+        <v>5</v>
+      </c>
+      <c r="P42" s="10">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="Q42" s="10">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
       <c r="R42" s="10" t="s">
         <v>264</v>
       </c>
@@ -2415,6 +3485,29 @@
       <c r="E43" s="7">
         <v>9073985531</v>
       </c>
+      <c r="K43" s="10">
+        <v>3</v>
+      </c>
+      <c r="L43" s="10">
+        <v>5</v>
+      </c>
+      <c r="M43" s="10">
+        <v>5</v>
+      </c>
+      <c r="N43" s="10">
+        <v>5</v>
+      </c>
+      <c r="O43" s="10">
+        <v>5</v>
+      </c>
+      <c r="P43" s="10">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="Q43" s="10">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
       <c r="R43" s="10" t="s">
         <v>264</v>
       </c>
@@ -2432,6 +3525,29 @@
       <c r="E44" s="7">
         <v>3324712220</v>
       </c>
+      <c r="K44" s="10">
+        <v>4</v>
+      </c>
+      <c r="L44" s="10">
+        <v>3</v>
+      </c>
+      <c r="M44" s="10">
+        <v>4</v>
+      </c>
+      <c r="N44" s="10">
+        <v>4</v>
+      </c>
+      <c r="O44" s="10">
+        <v>4</v>
+      </c>
+      <c r="P44" s="10">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="Q44" s="10">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
       <c r="R44" s="10" t="s">
         <v>264</v>
       </c>
@@ -2449,6 +3565,29 @@
       <c r="E45" s="7">
         <v>3324131158</v>
       </c>
+      <c r="K45" s="10">
+        <v>3</v>
+      </c>
+      <c r="L45" s="10">
+        <v>3</v>
+      </c>
+      <c r="M45" s="10">
+        <v>3</v>
+      </c>
+      <c r="N45" s="10">
+        <v>3</v>
+      </c>
+      <c r="O45" s="10">
+        <v>2</v>
+      </c>
+      <c r="P45" s="10">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="Q45" s="10">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
       <c r="R45" s="10" t="s">
         <v>264</v>
       </c>
@@ -2463,6 +3602,29 @@
       <c r="E46" s="7">
         <v>9836242629</v>
       </c>
+      <c r="K46" s="10">
+        <v>4</v>
+      </c>
+      <c r="L46" s="10">
+        <v>3</v>
+      </c>
+      <c r="M46" s="10">
+        <v>3</v>
+      </c>
+      <c r="N46" s="10">
+        <v>3</v>
+      </c>
+      <c r="O46" s="10">
+        <v>2</v>
+      </c>
+      <c r="P46" s="10">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="Q46" s="10">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
       <c r="R46" s="10" t="s">
         <v>264</v>
       </c>
@@ -2483,6 +3645,29 @@
       <c r="E47" s="7" t="s">
         <v>102</v>
       </c>
+      <c r="K47" s="10">
+        <v>3</v>
+      </c>
+      <c r="L47" s="10">
+        <v>4</v>
+      </c>
+      <c r="M47" s="10">
+        <v>4</v>
+      </c>
+      <c r="N47" s="10">
+        <v>4</v>
+      </c>
+      <c r="O47" s="10">
+        <v>4</v>
+      </c>
+      <c r="P47" s="10">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="Q47" s="10">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
       <c r="R47" s="10" t="s">
         <v>264</v>
       </c>
@@ -2503,6 +3688,29 @@
       <c r="E48" s="7">
         <v>9051973905</v>
       </c>
+      <c r="K48" s="10">
+        <v>2</v>
+      </c>
+      <c r="L48" s="10">
+        <v>4</v>
+      </c>
+      <c r="M48" s="10">
+        <v>5</v>
+      </c>
+      <c r="N48" s="10">
+        <v>5</v>
+      </c>
+      <c r="O48" s="10">
+        <v>4</v>
+      </c>
+      <c r="P48" s="10">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="Q48" s="10">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
       <c r="R48" s="10" t="s">
         <v>264</v>
       </c>
@@ -2523,6 +3731,29 @@
       <c r="E49" s="7">
         <v>9674850783</v>
       </c>
+      <c r="K49" s="10">
+        <v>2</v>
+      </c>
+      <c r="L49" s="10">
+        <v>3</v>
+      </c>
+      <c r="M49" s="10">
+        <v>5</v>
+      </c>
+      <c r="N49" s="10">
+        <v>3</v>
+      </c>
+      <c r="O49" s="10">
+        <v>3</v>
+      </c>
+      <c r="P49" s="10">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="Q49" s="10">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
       <c r="R49" s="10" t="s">
         <v>264</v>
       </c>
@@ -2543,6 +3774,29 @@
       <c r="E50" s="7">
         <v>9674111783</v>
       </c>
+      <c r="K50" s="10">
+        <v>4</v>
+      </c>
+      <c r="L50" s="10">
+        <v>2</v>
+      </c>
+      <c r="M50" s="10">
+        <v>3</v>
+      </c>
+      <c r="N50" s="10">
+        <v>3</v>
+      </c>
+      <c r="O50" s="10">
+        <v>1</v>
+      </c>
+      <c r="P50" s="10">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="Q50" s="10">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
       <c r="R50" s="10" t="s">
         <v>264</v>
       </c>
@@ -2563,6 +3817,29 @@
       <c r="E51" s="7">
         <v>33218260082</v>
       </c>
+      <c r="K51" s="10">
+        <v>2</v>
+      </c>
+      <c r="L51" s="10">
+        <v>4</v>
+      </c>
+      <c r="M51" s="10">
+        <v>5</v>
+      </c>
+      <c r="N51" s="10">
+        <v>4</v>
+      </c>
+      <c r="O51" s="10">
+        <v>3</v>
+      </c>
+      <c r="P51" s="10">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="Q51" s="10">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
       <c r="R51" s="10" t="s">
         <v>264</v>
       </c>
@@ -2583,6 +3860,29 @@
       <c r="E52" s="7">
         <v>3322879202</v>
       </c>
+      <c r="K52" s="10">
+        <v>3</v>
+      </c>
+      <c r="L52" s="10">
+        <v>5</v>
+      </c>
+      <c r="M52" s="10">
+        <v>5</v>
+      </c>
+      <c r="N52" s="10">
+        <v>5</v>
+      </c>
+      <c r="O52" s="10">
+        <v>4</v>
+      </c>
+      <c r="P52" s="10">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="Q52" s="10">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
       <c r="R52" s="10" t="s">
         <v>264</v>
       </c>
@@ -2603,6 +3903,29 @@
       <c r="E53" s="7">
         <v>3322841546</v>
       </c>
+      <c r="K53" s="10">
+        <v>3</v>
+      </c>
+      <c r="L53" s="10">
+        <v>5</v>
+      </c>
+      <c r="M53" s="10">
+        <v>5</v>
+      </c>
+      <c r="N53" s="10">
+        <v>5</v>
+      </c>
+      <c r="O53" s="10">
+        <v>5</v>
+      </c>
+      <c r="P53" s="10">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="Q53" s="10">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
       <c r="R53" s="10" t="s">
         <v>264</v>
       </c>
@@ -2623,6 +3946,29 @@
       <c r="E54" s="7">
         <v>3322484593</v>
       </c>
+      <c r="K54" s="10">
+        <v>3</v>
+      </c>
+      <c r="L54" s="10">
+        <v>4</v>
+      </c>
+      <c r="M54" s="10">
+        <v>4</v>
+      </c>
+      <c r="N54" s="10">
+        <v>4</v>
+      </c>
+      <c r="O54" s="10">
+        <v>4</v>
+      </c>
+      <c r="P54" s="10">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="Q54" s="10">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
       <c r="R54" s="10" t="s">
         <v>264</v>
       </c>
@@ -2643,6 +3989,29 @@
       <c r="E55" s="7">
         <v>3322297741</v>
       </c>
+      <c r="K55" s="10">
+        <v>3</v>
+      </c>
+      <c r="L55" s="10">
+        <v>4</v>
+      </c>
+      <c r="M55" s="10">
+        <v>4</v>
+      </c>
+      <c r="N55" s="10">
+        <v>4</v>
+      </c>
+      <c r="O55" s="10">
+        <v>3</v>
+      </c>
+      <c r="P55" s="10">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="Q55" s="10">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
       <c r="R55" s="10" t="s">
         <v>264</v>
       </c>
@@ -2663,6 +4032,29 @@
       <c r="E56" s="7">
         <v>3324793241</v>
       </c>
+      <c r="K56" s="10">
+        <v>2</v>
+      </c>
+      <c r="L56" s="10">
+        <v>3</v>
+      </c>
+      <c r="M56" s="10">
+        <v>4</v>
+      </c>
+      <c r="N56" s="10">
+        <v>3</v>
+      </c>
+      <c r="O56" s="10">
+        <v>4</v>
+      </c>
+      <c r="P56" s="10">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="Q56" s="10">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
       <c r="R56" s="10" t="s">
         <v>264</v>
       </c>
@@ -2683,6 +4075,29 @@
       <c r="E57" s="7">
         <v>3324344455</v>
       </c>
+      <c r="K57" s="10">
+        <v>3</v>
+      </c>
+      <c r="L57" s="10">
+        <v>3</v>
+      </c>
+      <c r="M57" s="10">
+        <v>3</v>
+      </c>
+      <c r="N57" s="10">
+        <v>3</v>
+      </c>
+      <c r="O57" s="10">
+        <v>2</v>
+      </c>
+      <c r="P57" s="10">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="Q57" s="10">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
       <c r="R57" s="10" t="s">
         <v>264</v>
       </c>
@@ -2703,6 +4118,29 @@
       <c r="E58" s="7">
         <v>3340083093</v>
       </c>
+      <c r="K58" s="10">
+        <v>3</v>
+      </c>
+      <c r="L58" s="10">
+        <v>3</v>
+      </c>
+      <c r="M58" s="10">
+        <v>3</v>
+      </c>
+      <c r="N58" s="10">
+        <v>2</v>
+      </c>
+      <c r="O58" s="10">
+        <v>2</v>
+      </c>
+      <c r="P58" s="10">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="Q58" s="10">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
       <c r="R58" s="10" t="s">
         <v>264</v>
       </c>
@@ -2723,6 +4161,29 @@
       <c r="E59" s="7">
         <v>3324618002</v>
       </c>
+      <c r="K59" s="10">
+        <v>2</v>
+      </c>
+      <c r="L59" s="10">
+        <v>3</v>
+      </c>
+      <c r="M59" s="10">
+        <v>4</v>
+      </c>
+      <c r="N59" s="10">
+        <v>4</v>
+      </c>
+      <c r="O59" s="10">
+        <v>3</v>
+      </c>
+      <c r="P59" s="10">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="Q59" s="10">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
       <c r="R59" s="10" t="s">
         <v>264</v>
       </c>
@@ -2743,6 +4204,29 @@
       <c r="E60" s="7" t="s">
         <v>127</v>
       </c>
+      <c r="K60" s="10">
+        <v>2</v>
+      </c>
+      <c r="L60" s="10">
+        <v>3</v>
+      </c>
+      <c r="M60" s="10">
+        <v>3</v>
+      </c>
+      <c r="N60" s="10">
+        <v>4</v>
+      </c>
+      <c r="O60" s="10">
+        <v>4</v>
+      </c>
+      <c r="P60" s="10">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="Q60" s="10">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
       <c r="R60" s="10" t="s">
         <v>264</v>
       </c>
@@ -2763,6 +4247,29 @@
       <c r="E61" s="7">
         <v>3324569090</v>
       </c>
+      <c r="K61" s="10">
+        <v>4</v>
+      </c>
+      <c r="L61" s="10">
+        <v>5</v>
+      </c>
+      <c r="M61" s="10">
+        <v>5</v>
+      </c>
+      <c r="N61" s="10">
+        <v>5</v>
+      </c>
+      <c r="O61" s="10">
+        <v>5</v>
+      </c>
+      <c r="P61" s="10">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="Q61" s="10">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
       <c r="R61" s="10" t="s">
         <v>264</v>
       </c>
@@ -2783,6 +4290,29 @@
       <c r="E62" s="7">
         <v>3322233062</v>
       </c>
+      <c r="K62" s="10">
+        <v>4</v>
+      </c>
+      <c r="L62" s="10">
+        <v>4</v>
+      </c>
+      <c r="M62" s="10">
+        <v>4</v>
+      </c>
+      <c r="N62" s="10">
+        <v>4</v>
+      </c>
+      <c r="O62" s="10">
+        <v>4</v>
+      </c>
+      <c r="P62" s="10">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="Q62" s="10">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
       <c r="R62" s="10" t="s">
         <v>264</v>
       </c>
@@ -2803,6 +4333,29 @@
       <c r="E63" s="7" t="s">
         <v>134</v>
       </c>
+      <c r="K63" s="10">
+        <v>3</v>
+      </c>
+      <c r="L63" s="10">
+        <v>4</v>
+      </c>
+      <c r="M63" s="10">
+        <v>3</v>
+      </c>
+      <c r="N63" s="10">
+        <v>5</v>
+      </c>
+      <c r="O63" s="10">
+        <v>3</v>
+      </c>
+      <c r="P63" s="10">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="Q63" s="10">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
       <c r="R63" s="10" t="s">
         <v>264</v>
       </c>
@@ -2823,6 +4376,29 @@
       <c r="E64" s="7">
         <v>3324793600</v>
       </c>
+      <c r="K64" s="10">
+        <v>4</v>
+      </c>
+      <c r="L64" s="10">
+        <v>5</v>
+      </c>
+      <c r="M64" s="10">
+        <v>5</v>
+      </c>
+      <c r="N64" s="10">
+        <v>5</v>
+      </c>
+      <c r="O64" s="10">
+        <v>5</v>
+      </c>
+      <c r="P64" s="10">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="Q64" s="10">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
       <c r="R64" s="10" t="s">
         <v>264</v>
       </c>
@@ -2843,6 +4419,29 @@
       <c r="E65" s="7">
         <v>3324866629</v>
       </c>
+      <c r="K65" s="10">
+        <v>3</v>
+      </c>
+      <c r="L65" s="10">
+        <v>3</v>
+      </c>
+      <c r="M65" s="10">
+        <v>3</v>
+      </c>
+      <c r="N65" s="10">
+        <v>5</v>
+      </c>
+      <c r="O65" s="10">
+        <v>3</v>
+      </c>
+      <c r="P65" s="10">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="Q65" s="10">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
       <c r="R65" s="10" t="s">
         <v>264</v>
       </c>
@@ -2863,6 +4462,29 @@
       <c r="E66" s="7">
         <v>3322848038</v>
       </c>
+      <c r="K66" s="10">
+        <v>3</v>
+      </c>
+      <c r="L66" s="10">
+        <v>3</v>
+      </c>
+      <c r="M66" s="10">
+        <v>4</v>
+      </c>
+      <c r="N66" s="10">
+        <v>4</v>
+      </c>
+      <c r="O66" s="10">
+        <v>2</v>
+      </c>
+      <c r="P66" s="10">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="Q66" s="10">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
       <c r="R66" s="10" t="s">
         <v>264</v>
       </c>
@@ -2883,6 +4505,29 @@
       <c r="E67" s="7">
         <v>905188888</v>
       </c>
+      <c r="K67" s="10">
+        <v>0</v>
+      </c>
+      <c r="L67" s="10">
+        <v>0</v>
+      </c>
+      <c r="M67" s="10">
+        <v>0</v>
+      </c>
+      <c r="N67" s="10">
+        <v>0</v>
+      </c>
+      <c r="O67" s="10">
+        <v>0</v>
+      </c>
+      <c r="P67" s="10">
+        <f t="shared" ref="P67:P122" si="2">SUM(K67:O67)</f>
+        <v>0</v>
+      </c>
+      <c r="Q67" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="R67" s="10" t="s">
         <v>264</v>
       </c>
@@ -2903,6 +4548,29 @@
       <c r="E68" s="7">
         <v>7596949952</v>
       </c>
+      <c r="K68" s="10">
+        <v>0</v>
+      </c>
+      <c r="L68" s="10">
+        <v>0</v>
+      </c>
+      <c r="M68" s="10">
+        <v>0</v>
+      </c>
+      <c r="N68" s="10">
+        <v>0</v>
+      </c>
+      <c r="O68" s="10">
+        <v>0</v>
+      </c>
+      <c r="P68" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q68" s="10">
+        <f t="shared" ref="Q68:Q122" si="3">ROUND(P68/5,0)</f>
+        <v>0</v>
+      </c>
       <c r="R68" s="10" t="s">
         <v>264</v>
       </c>
@@ -2923,6 +4591,29 @@
       <c r="E69" s="7">
         <v>7478196910</v>
       </c>
+      <c r="K69" s="10">
+        <v>0</v>
+      </c>
+      <c r="L69" s="10">
+        <v>0</v>
+      </c>
+      <c r="M69" s="10">
+        <v>0</v>
+      </c>
+      <c r="N69" s="10">
+        <v>0</v>
+      </c>
+      <c r="O69" s="10">
+        <v>0</v>
+      </c>
+      <c r="P69" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q69" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="R69" s="10" t="s">
         <v>264</v>
       </c>
@@ -2943,6 +4634,29 @@
       <c r="E70" s="7">
         <v>7044447761</v>
       </c>
+      <c r="K70" s="10">
+        <v>0</v>
+      </c>
+      <c r="L70" s="10">
+        <v>0</v>
+      </c>
+      <c r="M70" s="10">
+        <v>0</v>
+      </c>
+      <c r="N70" s="10">
+        <v>0</v>
+      </c>
+      <c r="O70" s="10">
+        <v>0</v>
+      </c>
+      <c r="P70" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q70" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="R70" s="10" t="s">
         <v>264</v>
       </c>
@@ -2963,6 +4677,29 @@
       <c r="E71" s="7">
         <v>7059600647</v>
       </c>
+      <c r="K71" s="10">
+        <v>0</v>
+      </c>
+      <c r="L71" s="10">
+        <v>0</v>
+      </c>
+      <c r="M71" s="10">
+        <v>0</v>
+      </c>
+      <c r="N71" s="10">
+        <v>0</v>
+      </c>
+      <c r="O71" s="10">
+        <v>0</v>
+      </c>
+      <c r="P71" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q71" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="R71" s="10" t="s">
         <v>264</v>
       </c>
@@ -2983,6 +4720,29 @@
       <c r="E72" s="7">
         <v>3340072444</v>
       </c>
+      <c r="K72" s="10">
+        <v>0</v>
+      </c>
+      <c r="L72" s="10">
+        <v>0</v>
+      </c>
+      <c r="M72" s="10">
+        <v>0</v>
+      </c>
+      <c r="N72" s="10">
+        <v>0</v>
+      </c>
+      <c r="O72" s="10">
+        <v>0</v>
+      </c>
+      <c r="P72" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q72" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="R72" s="10" t="s">
         <v>264</v>
       </c>
@@ -3003,6 +4763,29 @@
       <c r="E73" s="7">
         <v>9903102957</v>
       </c>
+      <c r="K73" s="10">
+        <v>0</v>
+      </c>
+      <c r="L73" s="10">
+        <v>0</v>
+      </c>
+      <c r="M73" s="10">
+        <v>0</v>
+      </c>
+      <c r="N73" s="10">
+        <v>0</v>
+      </c>
+      <c r="O73" s="10">
+        <v>0</v>
+      </c>
+      <c r="P73" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q73" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="R73" s="10" t="s">
         <v>264</v>
       </c>
@@ -3020,6 +4803,29 @@
       <c r="E74" s="7">
         <v>7605080650</v>
       </c>
+      <c r="K74" s="10">
+        <v>0</v>
+      </c>
+      <c r="L74" s="10">
+        <v>0</v>
+      </c>
+      <c r="M74" s="10">
+        <v>0</v>
+      </c>
+      <c r="N74" s="10">
+        <v>0</v>
+      </c>
+      <c r="O74" s="10">
+        <v>0</v>
+      </c>
+      <c r="P74" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q74" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="R74" s="10" t="s">
         <v>264</v>
       </c>
@@ -3040,6 +4846,29 @@
       <c r="E75" s="7">
         <v>3324752135</v>
       </c>
+      <c r="K75" s="10">
+        <v>0</v>
+      </c>
+      <c r="L75" s="10">
+        <v>0</v>
+      </c>
+      <c r="M75" s="10">
+        <v>0</v>
+      </c>
+      <c r="N75" s="10">
+        <v>0</v>
+      </c>
+      <c r="O75" s="10">
+        <v>0</v>
+      </c>
+      <c r="P75" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q75" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="R75" s="10" t="s">
         <v>264</v>
       </c>
@@ -3057,6 +4886,29 @@
       <c r="E76" s="7">
         <v>9674645471</v>
       </c>
+      <c r="K76" s="10">
+        <v>0</v>
+      </c>
+      <c r="L76" s="10">
+        <v>0</v>
+      </c>
+      <c r="M76" s="10">
+        <v>0</v>
+      </c>
+      <c r="N76" s="10">
+        <v>0</v>
+      </c>
+      <c r="O76" s="10">
+        <v>0</v>
+      </c>
+      <c r="P76" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q76" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="R76" s="10" t="s">
         <v>264</v>
       </c>
@@ -3071,6 +4923,29 @@
       <c r="E77" s="7">
         <v>9073681886</v>
       </c>
+      <c r="K77" s="10">
+        <v>0</v>
+      </c>
+      <c r="L77" s="10">
+        <v>0</v>
+      </c>
+      <c r="M77" s="10">
+        <v>0</v>
+      </c>
+      <c r="N77" s="10">
+        <v>0</v>
+      </c>
+      <c r="O77" s="10">
+        <v>0</v>
+      </c>
+      <c r="P77" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q77" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="R77" s="10" t="s">
         <v>264</v>
       </c>
@@ -3091,6 +4966,29 @@
       <c r="E78" s="7">
         <v>3324316997</v>
       </c>
+      <c r="K78" s="10">
+        <v>0</v>
+      </c>
+      <c r="L78" s="10">
+        <v>0</v>
+      </c>
+      <c r="M78" s="10">
+        <v>0</v>
+      </c>
+      <c r="N78" s="10">
+        <v>0</v>
+      </c>
+      <c r="O78" s="10">
+        <v>0</v>
+      </c>
+      <c r="P78" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q78" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="R78" s="10" t="s">
         <v>264</v>
       </c>
@@ -3111,6 +5009,29 @@
       <c r="E79" s="7">
         <v>3322291779</v>
       </c>
+      <c r="K79" s="10">
+        <v>0</v>
+      </c>
+      <c r="L79" s="10">
+        <v>0</v>
+      </c>
+      <c r="M79" s="10">
+        <v>0</v>
+      </c>
+      <c r="N79" s="10">
+        <v>0</v>
+      </c>
+      <c r="O79" s="10">
+        <v>0</v>
+      </c>
+      <c r="P79" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q79" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="R79" s="10" t="s">
         <v>264</v>
       </c>
@@ -3131,6 +5052,29 @@
       <c r="E80" s="7">
         <v>3323215151</v>
       </c>
+      <c r="K80" s="10">
+        <v>0</v>
+      </c>
+      <c r="L80" s="10">
+        <v>0</v>
+      </c>
+      <c r="M80" s="10">
+        <v>0</v>
+      </c>
+      <c r="N80" s="10">
+        <v>0</v>
+      </c>
+      <c r="O80" s="10">
+        <v>0</v>
+      </c>
+      <c r="P80" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q80" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="R80" s="10" t="s">
         <v>264</v>
       </c>
@@ -3151,6 +5095,29 @@
       <c r="E81" s="7">
         <v>3323342404</v>
       </c>
+      <c r="K81" s="10">
+        <v>0</v>
+      </c>
+      <c r="L81" s="10">
+        <v>0</v>
+      </c>
+      <c r="M81" s="10">
+        <v>0</v>
+      </c>
+      <c r="N81" s="10">
+        <v>0</v>
+      </c>
+      <c r="O81" s="10">
+        <v>0</v>
+      </c>
+      <c r="P81" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q81" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="R81" s="10" t="s">
         <v>264</v>
       </c>
@@ -3168,6 +5135,29 @@
       <c r="E82" s="7" t="s">
         <v>169</v>
       </c>
+      <c r="K82" s="10">
+        <v>0</v>
+      </c>
+      <c r="L82" s="10">
+        <v>0</v>
+      </c>
+      <c r="M82" s="10">
+        <v>0</v>
+      </c>
+      <c r="N82" s="10">
+        <v>0</v>
+      </c>
+      <c r="O82" s="10">
+        <v>0</v>
+      </c>
+      <c r="P82" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q82" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="R82" s="10" t="s">
         <v>264</v>
       </c>
@@ -3185,6 +5175,29 @@
       <c r="E83" s="7" t="s">
         <v>171</v>
       </c>
+      <c r="K83" s="10">
+        <v>0</v>
+      </c>
+      <c r="L83" s="10">
+        <v>0</v>
+      </c>
+      <c r="M83" s="10">
+        <v>0</v>
+      </c>
+      <c r="N83" s="10">
+        <v>0</v>
+      </c>
+      <c r="O83" s="10">
+        <v>0</v>
+      </c>
+      <c r="P83" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q83" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="R83" s="10" t="s">
         <v>264</v>
       </c>
@@ -3202,6 +5215,29 @@
       <c r="E84" s="7">
         <v>9606279184</v>
       </c>
+      <c r="K84" s="10">
+        <v>0</v>
+      </c>
+      <c r="L84" s="10">
+        <v>0</v>
+      </c>
+      <c r="M84" s="10">
+        <v>0</v>
+      </c>
+      <c r="N84" s="10">
+        <v>0</v>
+      </c>
+      <c r="O84" s="10">
+        <v>0</v>
+      </c>
+      <c r="P84" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q84" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="R84" s="10" t="s">
         <v>264</v>
       </c>
@@ -3222,6 +5258,29 @@
       <c r="E85" s="7">
         <v>8777867589</v>
       </c>
+      <c r="K85" s="10">
+        <v>0</v>
+      </c>
+      <c r="L85" s="10">
+        <v>0</v>
+      </c>
+      <c r="M85" s="10">
+        <v>0</v>
+      </c>
+      <c r="N85" s="10">
+        <v>0</v>
+      </c>
+      <c r="O85" s="10">
+        <v>0</v>
+      </c>
+      <c r="P85" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q85" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="R85" s="10" t="s">
         <v>264</v>
       </c>
@@ -3239,6 +5298,29 @@
       <c r="E86" s="7">
         <v>8017672075</v>
       </c>
+      <c r="K86" s="10">
+        <v>0</v>
+      </c>
+      <c r="L86" s="10">
+        <v>0</v>
+      </c>
+      <c r="M86" s="10">
+        <v>0</v>
+      </c>
+      <c r="N86" s="10">
+        <v>0</v>
+      </c>
+      <c r="O86" s="10">
+        <v>0</v>
+      </c>
+      <c r="P86" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q86" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="R86" s="10" t="s">
         <v>264</v>
       </c>
@@ -3256,6 +5338,29 @@
       <c r="E87" s="7">
         <v>3324492810</v>
       </c>
+      <c r="K87" s="10">
+        <v>0</v>
+      </c>
+      <c r="L87" s="10">
+        <v>0</v>
+      </c>
+      <c r="M87" s="10">
+        <v>0</v>
+      </c>
+      <c r="N87" s="10">
+        <v>0</v>
+      </c>
+      <c r="O87" s="10">
+        <v>0</v>
+      </c>
+      <c r="P87" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q87" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="R87" s="10" t="s">
         <v>264</v>
       </c>
@@ -3276,6 +5381,29 @@
       <c r="E88" s="7">
         <v>3324967196</v>
       </c>
+      <c r="K88" s="10">
+        <v>0</v>
+      </c>
+      <c r="L88" s="10">
+        <v>0</v>
+      </c>
+      <c r="M88" s="10">
+        <v>0</v>
+      </c>
+      <c r="N88" s="10">
+        <v>0</v>
+      </c>
+      <c r="O88" s="10">
+        <v>0</v>
+      </c>
+      <c r="P88" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q88" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="R88" s="10" t="s">
         <v>264</v>
       </c>
@@ -3296,6 +5424,29 @@
       <c r="E89" s="7">
         <v>9830701347</v>
       </c>
+      <c r="K89" s="10">
+        <v>0</v>
+      </c>
+      <c r="L89" s="10">
+        <v>0</v>
+      </c>
+      <c r="M89" s="10">
+        <v>0</v>
+      </c>
+      <c r="N89" s="10">
+        <v>0</v>
+      </c>
+      <c r="O89" s="10">
+        <v>0</v>
+      </c>
+      <c r="P89" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q89" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="R89" s="10" t="s">
         <v>264</v>
       </c>
@@ -3313,6 +5464,29 @@
       <c r="E90" s="7">
         <v>3324961723</v>
       </c>
+      <c r="K90" s="10">
+        <v>0</v>
+      </c>
+      <c r="L90" s="10">
+        <v>0</v>
+      </c>
+      <c r="M90" s="10">
+        <v>0</v>
+      </c>
+      <c r="N90" s="10">
+        <v>0</v>
+      </c>
+      <c r="O90" s="10">
+        <v>0</v>
+      </c>
+      <c r="P90" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q90" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="R90" s="10" t="s">
         <v>264</v>
       </c>
@@ -3333,6 +5507,29 @@
       <c r="E91" s="7">
         <v>9007792852</v>
       </c>
+      <c r="K91" s="10">
+        <v>0</v>
+      </c>
+      <c r="L91" s="10">
+        <v>0</v>
+      </c>
+      <c r="M91" s="10">
+        <v>0</v>
+      </c>
+      <c r="N91" s="10">
+        <v>0</v>
+      </c>
+      <c r="O91" s="10">
+        <v>0</v>
+      </c>
+      <c r="P91" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q91" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="R91" s="10" t="s">
         <v>264</v>
       </c>
@@ -3350,6 +5547,29 @@
       <c r="E92" s="7">
         <v>8902765583</v>
       </c>
+      <c r="K92" s="10">
+        <v>0</v>
+      </c>
+      <c r="L92" s="10">
+        <v>0</v>
+      </c>
+      <c r="M92" s="10">
+        <v>0</v>
+      </c>
+      <c r="N92" s="10">
+        <v>0</v>
+      </c>
+      <c r="O92" s="10">
+        <v>0</v>
+      </c>
+      <c r="P92" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q92" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="R92" s="10" t="s">
         <v>264</v>
       </c>
@@ -3367,6 +5587,29 @@
       <c r="E93" s="7">
         <v>9331866252</v>
       </c>
+      <c r="K93" s="10">
+        <v>0</v>
+      </c>
+      <c r="L93" s="10">
+        <v>0</v>
+      </c>
+      <c r="M93" s="10">
+        <v>0</v>
+      </c>
+      <c r="N93" s="10">
+        <v>0</v>
+      </c>
+      <c r="O93" s="10">
+        <v>0</v>
+      </c>
+      <c r="P93" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q93" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="R93" s="10" t="s">
         <v>264</v>
       </c>
@@ -3384,6 +5627,29 @@
       <c r="E94" s="7">
         <v>9903540099</v>
       </c>
+      <c r="K94" s="10">
+        <v>0</v>
+      </c>
+      <c r="L94" s="10">
+        <v>0</v>
+      </c>
+      <c r="M94" s="10">
+        <v>0</v>
+      </c>
+      <c r="N94" s="10">
+        <v>0</v>
+      </c>
+      <c r="O94" s="10">
+        <v>0</v>
+      </c>
+      <c r="P94" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q94" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="R94" s="10" t="s">
         <v>264</v>
       </c>
@@ -3401,6 +5667,29 @@
       <c r="E95" s="7">
         <v>8336998663</v>
       </c>
+      <c r="K95" s="10">
+        <v>0</v>
+      </c>
+      <c r="L95" s="10">
+        <v>0</v>
+      </c>
+      <c r="M95" s="10">
+        <v>0</v>
+      </c>
+      <c r="N95" s="10">
+        <v>0</v>
+      </c>
+      <c r="O95" s="10">
+        <v>0</v>
+      </c>
+      <c r="P95" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q95" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="R95" s="10" t="s">
         <v>264</v>
       </c>
@@ -3418,6 +5707,29 @@
       <c r="E96" s="7">
         <v>9339527506</v>
       </c>
+      <c r="K96" s="10">
+        <v>0</v>
+      </c>
+      <c r="L96" s="10">
+        <v>0</v>
+      </c>
+      <c r="M96" s="10">
+        <v>0</v>
+      </c>
+      <c r="N96" s="10">
+        <v>0</v>
+      </c>
+      <c r="O96" s="10">
+        <v>0</v>
+      </c>
+      <c r="P96" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q96" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="R96" s="10" t="s">
         <v>264</v>
       </c>
@@ -3432,11 +5744,31 @@
       <c r="E97" s="7">
         <v>9903312630</v>
       </c>
-      <c r="J97" s="1" t="s">
-        <v>211</v>
+      <c r="K97" s="10">
+        <v>0</v>
+      </c>
+      <c r="L97" s="10">
+        <v>0</v>
+      </c>
+      <c r="M97" s="10">
+        <v>0</v>
+      </c>
+      <c r="N97" s="10">
+        <v>0</v>
+      </c>
+      <c r="O97" s="10">
+        <v>0</v>
+      </c>
+      <c r="P97" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q97" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="R97" s="10" t="s">
-        <v>252</v>
+        <v>264</v>
       </c>
     </row>
     <row r="98" spans="1:18" x14ac:dyDescent="0.3">
@@ -3449,6 +5781,29 @@
       <c r="E98" s="7">
         <v>9836747400</v>
       </c>
+      <c r="K98" s="10">
+        <v>0</v>
+      </c>
+      <c r="L98" s="10">
+        <v>0</v>
+      </c>
+      <c r="M98" s="10">
+        <v>0</v>
+      </c>
+      <c r="N98" s="10">
+        <v>0</v>
+      </c>
+      <c r="O98" s="10">
+        <v>0</v>
+      </c>
+      <c r="P98" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q98" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="R98" s="10" t="s">
         <v>264</v>
       </c>
@@ -3463,6 +5818,29 @@
       <c r="E99" s="7">
         <v>8100188019</v>
       </c>
+      <c r="K99" s="10">
+        <v>0</v>
+      </c>
+      <c r="L99" s="10">
+        <v>0</v>
+      </c>
+      <c r="M99" s="10">
+        <v>0</v>
+      </c>
+      <c r="N99" s="10">
+        <v>0</v>
+      </c>
+      <c r="O99" s="10">
+        <v>0</v>
+      </c>
+      <c r="P99" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q99" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="R99" s="10" t="s">
         <v>264</v>
       </c>
@@ -3477,6 +5855,29 @@
       <c r="E100" s="7" t="s">
         <v>197</v>
       </c>
+      <c r="K100" s="10">
+        <v>0</v>
+      </c>
+      <c r="L100" s="10">
+        <v>0</v>
+      </c>
+      <c r="M100" s="10">
+        <v>0</v>
+      </c>
+      <c r="N100" s="10">
+        <v>0</v>
+      </c>
+      <c r="O100" s="10">
+        <v>0</v>
+      </c>
+      <c r="P100" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q100" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="R100" s="10" t="s">
         <v>264</v>
       </c>
@@ -3491,6 +5892,29 @@
       <c r="E101" s="7" t="s">
         <v>198</v>
       </c>
+      <c r="K101" s="10">
+        <v>0</v>
+      </c>
+      <c r="L101" s="10">
+        <v>0</v>
+      </c>
+      <c r="M101" s="10">
+        <v>0</v>
+      </c>
+      <c r="N101" s="10">
+        <v>0</v>
+      </c>
+      <c r="O101" s="10">
+        <v>0</v>
+      </c>
+      <c r="P101" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q101" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="R101" s="10" t="s">
         <v>264</v>
       </c>
@@ -3505,6 +5929,29 @@
       <c r="E102" s="7" t="s">
         <v>201</v>
       </c>
+      <c r="K102" s="10">
+        <v>0</v>
+      </c>
+      <c r="L102" s="10">
+        <v>0</v>
+      </c>
+      <c r="M102" s="10">
+        <v>0</v>
+      </c>
+      <c r="N102" s="10">
+        <v>0</v>
+      </c>
+      <c r="O102" s="10">
+        <v>0</v>
+      </c>
+      <c r="P102" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q102" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="R102" s="10" t="s">
         <v>264</v>
       </c>
@@ -3519,6 +5966,29 @@
       <c r="E103" s="7" t="s">
         <v>202</v>
       </c>
+      <c r="K103" s="10">
+        <v>0</v>
+      </c>
+      <c r="L103" s="10">
+        <v>0</v>
+      </c>
+      <c r="M103" s="10">
+        <v>0</v>
+      </c>
+      <c r="N103" s="10">
+        <v>0</v>
+      </c>
+      <c r="O103" s="10">
+        <v>0</v>
+      </c>
+      <c r="P103" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q103" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="R103" s="10" t="s">
         <v>264</v>
       </c>
@@ -3533,6 +6003,29 @@
       <c r="E104" s="7" t="s">
         <v>203</v>
       </c>
+      <c r="K104" s="10">
+        <v>0</v>
+      </c>
+      <c r="L104" s="10">
+        <v>0</v>
+      </c>
+      <c r="M104" s="10">
+        <v>0</v>
+      </c>
+      <c r="N104" s="10">
+        <v>0</v>
+      </c>
+      <c r="O104" s="10">
+        <v>0</v>
+      </c>
+      <c r="P104" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q104" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="R104" s="10" t="s">
         <v>264</v>
       </c>
@@ -3547,6 +6040,29 @@
       <c r="E105" s="7" t="s">
         <v>204</v>
       </c>
+      <c r="K105" s="10">
+        <v>0</v>
+      </c>
+      <c r="L105" s="10">
+        <v>0</v>
+      </c>
+      <c r="M105" s="10">
+        <v>0</v>
+      </c>
+      <c r="N105" s="10">
+        <v>0</v>
+      </c>
+      <c r="O105" s="10">
+        <v>0</v>
+      </c>
+      <c r="P105" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q105" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="R105" s="10" t="s">
         <v>264</v>
       </c>
@@ -3561,6 +6077,29 @@
       <c r="E106" s="7" t="s">
         <v>205</v>
       </c>
+      <c r="K106" s="10">
+        <v>0</v>
+      </c>
+      <c r="L106" s="10">
+        <v>0</v>
+      </c>
+      <c r="M106" s="10">
+        <v>0</v>
+      </c>
+      <c r="N106" s="10">
+        <v>0</v>
+      </c>
+      <c r="O106" s="10">
+        <v>0</v>
+      </c>
+      <c r="P106" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q106" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="R106" s="10" t="s">
         <v>264</v>
       </c>
@@ -3575,6 +6114,29 @@
       <c r="E107" s="7" t="s">
         <v>206</v>
       </c>
+      <c r="K107" s="10">
+        <v>0</v>
+      </c>
+      <c r="L107" s="10">
+        <v>0</v>
+      </c>
+      <c r="M107" s="10">
+        <v>0</v>
+      </c>
+      <c r="N107" s="10">
+        <v>0</v>
+      </c>
+      <c r="O107" s="10">
+        <v>0</v>
+      </c>
+      <c r="P107" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q107" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="R107" s="10" t="s">
         <v>264</v>
       </c>
@@ -3589,6 +6151,29 @@
       <c r="E108" s="7" t="s">
         <v>208</v>
       </c>
+      <c r="K108" s="10">
+        <v>0</v>
+      </c>
+      <c r="L108" s="10">
+        <v>0</v>
+      </c>
+      <c r="M108" s="10">
+        <v>0</v>
+      </c>
+      <c r="N108" s="10">
+        <v>0</v>
+      </c>
+      <c r="O108" s="10">
+        <v>0</v>
+      </c>
+      <c r="P108" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q108" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="R108" s="10" t="s">
         <v>264</v>
       </c>
@@ -3603,6 +6188,29 @@
       <c r="E109" s="7" t="s">
         <v>210</v>
       </c>
+      <c r="K109" s="10">
+        <v>0</v>
+      </c>
+      <c r="L109" s="10">
+        <v>0</v>
+      </c>
+      <c r="M109" s="10">
+        <v>0</v>
+      </c>
+      <c r="N109" s="10">
+        <v>0</v>
+      </c>
+      <c r="O109" s="10">
+        <v>0</v>
+      </c>
+      <c r="P109" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q109" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="R109" s="10" t="s">
         <v>264</v>
       </c>
@@ -3617,6 +6225,29 @@
       <c r="E110" s="7" t="s">
         <v>213</v>
       </c>
+      <c r="K110" s="10">
+        <v>0</v>
+      </c>
+      <c r="L110" s="10">
+        <v>0</v>
+      </c>
+      <c r="M110" s="10">
+        <v>0</v>
+      </c>
+      <c r="N110" s="10">
+        <v>0</v>
+      </c>
+      <c r="O110" s="10">
+        <v>0</v>
+      </c>
+      <c r="P110" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q110" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="R110" s="10" t="s">
         <v>264</v>
       </c>
@@ -3631,6 +6262,29 @@
       <c r="E111" s="7" t="s">
         <v>215</v>
       </c>
+      <c r="K111" s="10">
+        <v>0</v>
+      </c>
+      <c r="L111" s="10">
+        <v>0</v>
+      </c>
+      <c r="M111" s="10">
+        <v>0</v>
+      </c>
+      <c r="N111" s="10">
+        <v>0</v>
+      </c>
+      <c r="O111" s="10">
+        <v>0</v>
+      </c>
+      <c r="P111" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q111" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="R111" s="10" t="s">
         <v>264</v>
       </c>
@@ -3645,6 +6299,29 @@
       <c r="E112" s="7" t="s">
         <v>217</v>
       </c>
+      <c r="K112" s="10">
+        <v>0</v>
+      </c>
+      <c r="L112" s="10">
+        <v>0</v>
+      </c>
+      <c r="M112" s="10">
+        <v>0</v>
+      </c>
+      <c r="N112" s="10">
+        <v>0</v>
+      </c>
+      <c r="O112" s="10">
+        <v>0</v>
+      </c>
+      <c r="P112" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q112" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="R112" s="10" t="s">
         <v>264</v>
       </c>
@@ -3659,6 +6336,29 @@
       <c r="E113" s="7" t="s">
         <v>219</v>
       </c>
+      <c r="K113" s="10">
+        <v>0</v>
+      </c>
+      <c r="L113" s="10">
+        <v>0</v>
+      </c>
+      <c r="M113" s="10">
+        <v>0</v>
+      </c>
+      <c r="N113" s="10">
+        <v>0</v>
+      </c>
+      <c r="O113" s="10">
+        <v>0</v>
+      </c>
+      <c r="P113" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q113" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="R113" s="10" t="s">
         <v>264</v>
       </c>
@@ -3673,6 +6373,29 @@
       <c r="E114" s="7" t="s">
         <v>221</v>
       </c>
+      <c r="K114" s="10">
+        <v>0</v>
+      </c>
+      <c r="L114" s="10">
+        <v>0</v>
+      </c>
+      <c r="M114" s="10">
+        <v>0</v>
+      </c>
+      <c r="N114" s="10">
+        <v>0</v>
+      </c>
+      <c r="O114" s="10">
+        <v>0</v>
+      </c>
+      <c r="P114" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q114" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="R114" s="10" t="s">
         <v>264</v>
       </c>
@@ -3687,6 +6410,29 @@
       <c r="E115" s="7" t="s">
         <v>223</v>
       </c>
+      <c r="K115" s="10">
+        <v>0</v>
+      </c>
+      <c r="L115" s="10">
+        <v>0</v>
+      </c>
+      <c r="M115" s="10">
+        <v>0</v>
+      </c>
+      <c r="N115" s="10">
+        <v>0</v>
+      </c>
+      <c r="O115" s="10">
+        <v>0</v>
+      </c>
+      <c r="P115" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q115" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="R115" s="10" t="s">
         <v>264</v>
       </c>
@@ -3701,6 +6447,29 @@
       <c r="E116" s="7" t="s">
         <v>225</v>
       </c>
+      <c r="K116" s="10">
+        <v>0</v>
+      </c>
+      <c r="L116" s="10">
+        <v>0</v>
+      </c>
+      <c r="M116" s="10">
+        <v>0</v>
+      </c>
+      <c r="N116" s="10">
+        <v>0</v>
+      </c>
+      <c r="O116" s="10">
+        <v>0</v>
+      </c>
+      <c r="P116" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q116" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="R116" s="10" t="s">
         <v>264</v>
       </c>
@@ -3715,6 +6484,29 @@
       <c r="E117" s="7" t="s">
         <v>227</v>
       </c>
+      <c r="K117" s="10">
+        <v>0</v>
+      </c>
+      <c r="L117" s="10">
+        <v>0</v>
+      </c>
+      <c r="M117" s="10">
+        <v>0</v>
+      </c>
+      <c r="N117" s="10">
+        <v>0</v>
+      </c>
+      <c r="O117" s="10">
+        <v>0</v>
+      </c>
+      <c r="P117" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q117" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="R117" s="10" t="s">
         <v>264</v>
       </c>
@@ -3729,6 +6521,29 @@
       <c r="E118" s="7" t="s">
         <v>229</v>
       </c>
+      <c r="K118" s="10">
+        <v>0</v>
+      </c>
+      <c r="L118" s="10">
+        <v>0</v>
+      </c>
+      <c r="M118" s="10">
+        <v>0</v>
+      </c>
+      <c r="N118" s="10">
+        <v>0</v>
+      </c>
+      <c r="O118" s="10">
+        <v>0</v>
+      </c>
+      <c r="P118" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q118" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="R118" s="10" t="s">
         <v>264</v>
       </c>
@@ -3743,6 +6558,29 @@
       <c r="E119" s="7" t="s">
         <v>230</v>
       </c>
+      <c r="K119" s="10">
+        <v>3</v>
+      </c>
+      <c r="L119" s="10">
+        <v>4</v>
+      </c>
+      <c r="M119" s="10">
+        <v>4</v>
+      </c>
+      <c r="N119" s="10">
+        <v>4</v>
+      </c>
+      <c r="O119" s="10">
+        <v>3</v>
+      </c>
+      <c r="P119" s="10">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="Q119" s="10">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
       <c r="R119" s="10" t="s">
         <v>264</v>
       </c>
@@ -3757,6 +6595,29 @@
       <c r="E120" s="7" t="s">
         <v>233</v>
       </c>
+      <c r="K120" s="10">
+        <v>1</v>
+      </c>
+      <c r="L120" s="10">
+        <v>4</v>
+      </c>
+      <c r="M120" s="10">
+        <v>4</v>
+      </c>
+      <c r="N120" s="10">
+        <v>4</v>
+      </c>
+      <c r="O120" s="10">
+        <v>3</v>
+      </c>
+      <c r="P120" s="10">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="Q120" s="10">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
       <c r="R120" s="10" t="s">
         <v>264</v>
       </c>
@@ -3771,6 +6632,29 @@
       <c r="E121" s="7" t="s">
         <v>235</v>
       </c>
+      <c r="K121" s="10">
+        <v>3</v>
+      </c>
+      <c r="L121" s="10">
+        <v>2</v>
+      </c>
+      <c r="M121" s="10">
+        <v>2</v>
+      </c>
+      <c r="N121" s="10">
+        <v>2</v>
+      </c>
+      <c r="O121" s="10">
+        <v>1</v>
+      </c>
+      <c r="P121" s="10">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="Q121" s="10">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
       <c r="R121" s="10" t="s">
         <v>264</v>
       </c>
@@ -3784,6 +6668,29 @@
       </c>
       <c r="E122" s="7" t="s">
         <v>237</v>
+      </c>
+      <c r="K122" s="10">
+        <v>1</v>
+      </c>
+      <c r="L122" s="10">
+        <v>3</v>
+      </c>
+      <c r="M122" s="10">
+        <v>3</v>
+      </c>
+      <c r="N122" s="10">
+        <v>2</v>
+      </c>
+      <c r="O122" s="10">
+        <v>2</v>
+      </c>
+      <c r="P122" s="10">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="Q122" s="10">
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="R122" s="10" t="s">
         <v>264</v>

</xml_diff>

<commit_message>
AI Workshop For Schools
AI Workshop For Schools
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Marketing/AI marketing/AI Workshop Schools.xlsx
+++ b/Offline/BusinessManagement/Marketing/AI marketing/AI Workshop Schools.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Marketing\AI marketing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5442D69-A5D0-436E-A91E-977747376A5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB67B7E-0FF8-426E-89CE-DB322D776A9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" tabRatio="540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="8" r:id="rId1"/>
@@ -20,10 +20,19 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'School-Details'!$A$1:$U$1</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -64,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="285">
   <si>
     <t>CBSE</t>
   </si>
@@ -919,6 +928,9 @@
   </si>
   <si>
     <t>Contact Person Designation</t>
+  </si>
+  <si>
+    <t>Debashish Nath</t>
   </si>
 </sst>
 </file>
@@ -1125,12 +1137,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1139,6 +1145,12 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1421,24 +1433,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DC48E2D-CE6A-43EF-B55A-B9B416B6A77B}">
-  <dimension ref="B2:L23"/>
+  <dimension ref="B2:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="21.53125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.53125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" customWidth="1"/>
-    <col min="10" max="10" width="10.86328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="12.1328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C2" s="16" t="s">
         <v>246</v>
       </c>
@@ -1447,12 +1459,12 @@
         <v>121</v>
       </c>
       <c r="J2" s="14"/>
-      <c r="K2" s="24" t="s">
+      <c r="K2" s="27" t="s">
         <v>211</v>
       </c>
-      <c r="L2" s="25"/>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="L2" s="28"/>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C3" s="16" t="s">
         <v>247</v>
       </c>
@@ -1470,7 +1482,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="J4" s="22">
         <v>45292</v>
       </c>
@@ -1481,7 +1493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C5" s="21" t="s">
         <v>248</v>
       </c>
@@ -1504,7 +1516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C6" s="14" t="s">
         <v>252</v>
       </c>
@@ -1529,7 +1541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C7" s="14" t="s">
         <v>254</v>
       </c>
@@ -1554,7 +1566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C8" s="14" t="s">
         <v>256</v>
       </c>
@@ -1579,7 +1591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C9" s="14" t="s">
         <v>258</v>
       </c>
@@ -1587,6 +1599,13 @@
         <f>COUNTIF('School-Details'!U:U,C9)</f>
         <v>0</v>
       </c>
+      <c r="F9" s="14" t="s">
+        <v>284</v>
+      </c>
+      <c r="G9" s="14">
+        <f>COUNTIF('School-Details'!M:M,F9)</f>
+        <v>0</v>
+      </c>
       <c r="J9" s="22">
         <v>45444</v>
       </c>
@@ -1597,7 +1616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C10" s="14" t="s">
         <v>260</v>
       </c>
@@ -1615,7 +1634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C11" s="14" t="s">
         <v>262</v>
       </c>
@@ -1633,7 +1652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C12" s="14" t="s">
         <v>264</v>
       </c>
@@ -1651,7 +1670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C13" s="14" t="s">
         <v>280</v>
       </c>
@@ -1669,7 +1688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="J14" s="22">
         <v>45597</v>
       </c>
@@ -1680,7 +1699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B15" s="23"/>
       <c r="C15" s="21" t="s">
         <v>275</v>
@@ -1698,7 +1717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B16" s="14" t="s">
         <v>273</v>
       </c>
@@ -1707,7 +1726,7 @@
       </c>
       <c r="D16" s="14">
         <f>COUNTIF('School-Details'!T:T,C16)</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J16" s="16" t="s">
         <v>245</v>
@@ -1721,27 +1740,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B17" s="14"/>
       <c r="C17" s="14">
         <v>4</v>
       </c>
       <c r="D17" s="14">
         <f>COUNTIF('School-Details'!T:T,C17)</f>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.45">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" s="14"/>
       <c r="C18" s="14" t="s">
         <v>276</v>
       </c>
       <c r="D18" s="14">
         <f>SUM(D16:D17)</f>
-        <v>43</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.45">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" s="14" t="s">
         <v>279</v>
       </c>
@@ -1750,20 +1769,20 @@
       </c>
       <c r="D19" s="14">
         <f>COUNTIF('School-Details'!T:T,C19)</f>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.45">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" s="14"/>
       <c r="C20" s="14" t="s">
         <v>278</v>
       </c>
       <c r="D20" s="14">
         <f>SUM(D19)</f>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.45">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" s="14" t="s">
         <v>274</v>
       </c>
@@ -1772,10 +1791,10 @@
       </c>
       <c r="D21" s="14">
         <f>COUNTIF('School-Details'!T:T,C21)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.45">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" s="14"/>
       <c r="C22" s="14">
         <v>1</v>
@@ -1785,14 +1804,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" s="14"/>
       <c r="C23" s="14" t="s">
         <v>277</v>
       </c>
       <c r="D23" s="14">
         <f>SUM(D21:D22)</f>
-        <v>2</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B24" s="14"/>
+      <c r="C24" s="16" t="s">
+        <v>245</v>
+      </c>
+      <c r="D24" s="16">
+        <f>D18+D20+D23</f>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1808,33 +1837,33 @@
   <dimension ref="A1:U122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T1" sqref="T1"/>
+      <selection pane="bottomRight" activeCell="N119" sqref="N119"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.6640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="25.6640625" style="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.1328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.3984375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.265625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.46484375" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.21875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" style="7" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="16" style="1" customWidth="1"/>
     <col min="10" max="11" width="11" style="1" customWidth="1"/>
     <col min="12" max="12" width="19.6640625" style="1" customWidth="1"/>
     <col min="13" max="13" width="13.33203125" style="1" customWidth="1"/>
     <col min="14" max="14" width="14" style="1" customWidth="1"/>
-    <col min="15" max="20" width="9.1328125" style="1"/>
-    <col min="21" max="21" width="20.53125" style="10" customWidth="1"/>
+    <col min="15" max="20" width="9.109375" style="1"/>
+    <col min="21" max="21" width="20.5546875" style="10" customWidth="1"/>
     <col min="22" max="22" width="13.6640625" style="1" customWidth="1"/>
-    <col min="23" max="16384" width="9.1328125" style="1"/>
+    <col min="23" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>1</v>
       </c>
@@ -1844,19 +1873,19 @@
       <c r="C1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="24" t="s">
         <v>39</v>
       </c>
       <c r="E1" s="18" t="s">
         <v>281</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="25" t="s">
         <v>6</v>
       </c>
       <c r="G1" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="24" t="s">
         <v>282</v>
       </c>
       <c r="I1" s="18" t="s">
@@ -1892,14 +1921,14 @@
       <c r="S1" s="20" t="s">
         <v>245</v>
       </c>
-      <c r="T1" s="28" t="s">
+      <c r="T1" s="26" t="s">
         <v>243</v>
       </c>
       <c r="U1" s="20" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1939,7 +1968,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1976,7 +2005,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2019,7 +2048,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2056,7 +2085,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2093,7 +2122,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2130,7 +2159,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2167,7 +2196,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -2207,7 +2236,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -2244,7 +2273,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -2281,7 +2310,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -2318,7 +2347,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -2355,7 +2384,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:21" ht="72" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -2392,7 +2421,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -2429,7 +2458,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -2466,7 +2495,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -2503,7 +2532,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -2540,7 +2569,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -2577,7 +2606,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -2617,7 +2646,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -2658,7 +2687,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -2699,7 +2728,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -2739,7 +2768,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -2780,7 +2809,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -2821,7 +2850,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -2862,7 +2891,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -2903,7 +2932,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -2940,7 +2969,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -2977,7 +3006,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -3018,7 +3047,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -3059,7 +3088,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -3100,7 +3129,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -3144,7 +3173,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -3184,7 +3213,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -3228,7 +3257,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -3271,7 +3300,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -3315,7 +3344,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -3355,7 +3384,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -3392,7 +3421,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -3432,7 +3461,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -3476,7 +3505,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -3520,7 +3549,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -3564,7 +3593,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -3604,7 +3633,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -3644,7 +3673,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -3681,7 +3710,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="47" spans="1:21" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -3725,7 +3754,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -3769,7 +3798,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -3813,7 +3842,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -3856,7 +3885,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -3900,7 +3929,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -3944,7 +3973,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -3988,7 +4017,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -4032,7 +4061,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -4076,7 +4105,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -4120,7 +4149,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -4164,7 +4193,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -4208,7 +4237,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -4252,7 +4281,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -4296,7 +4325,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -4340,7 +4369,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <v>61</v>
       </c>
@@ -4384,7 +4413,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="63" spans="1:21" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
         <v>62</v>
       </c>
@@ -4428,7 +4457,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <v>63</v>
       </c>
@@ -4472,7 +4501,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -4516,7 +4545,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
         <v>65</v>
       </c>
@@ -4560,7 +4589,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
         <v>66</v>
       </c>
@@ -4578,33 +4607,33 @@
         <v>905188888</v>
       </c>
       <c r="N67" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O67" s="10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P67" s="10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Q67" s="10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R67" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S67" s="10">
         <f t="shared" ref="S67:S122" si="2">SUM(N67:R67)</f>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="T67" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U67" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <v>67</v>
       </c>
@@ -4622,33 +4651,33 @@
         <v>7596949952</v>
       </c>
       <c r="N68" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O68" s="10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P68" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Q68" s="10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R68" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S68" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="T68" s="10">
         <f t="shared" ref="T68:T122" si="3">ROUND(S68/5,0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U68" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
         <v>68</v>
       </c>
@@ -4666,33 +4695,33 @@
         <v>7478196910</v>
       </c>
       <c r="N69" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O69" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P69" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Q69" s="10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R69" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S69" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="T69" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U69" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A70" s="2">
         <v>69</v>
       </c>
@@ -4710,33 +4739,33 @@
         <v>7044447761</v>
       </c>
       <c r="N70" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O70" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P70" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q70" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R70" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S70" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="T70" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U70" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A71" s="2">
         <v>70</v>
       </c>
@@ -4754,33 +4783,33 @@
         <v>7059600647</v>
       </c>
       <c r="N71" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O71" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P71" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q71" s="10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R71" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S71" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="T71" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U71" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A72" s="2">
         <v>71</v>
       </c>
@@ -4798,33 +4827,33 @@
         <v>3340072444</v>
       </c>
       <c r="N72" s="10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O72" s="10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P72" s="10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Q72" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R72" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S72" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="T72" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="U72" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A73" s="2">
         <v>72</v>
       </c>
@@ -4842,33 +4871,33 @@
         <v>9903102957</v>
       </c>
       <c r="N73" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O73" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P73" s="10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Q73" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R73" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S73" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="T73" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U73" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A74" s="2">
         <v>73</v>
       </c>
@@ -4882,33 +4911,33 @@
         <v>7605080650</v>
       </c>
       <c r="N74" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O74" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P74" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Q74" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R74" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S74" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="T74" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U74" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A75" s="2">
         <v>74</v>
       </c>
@@ -4926,33 +4955,33 @@
         <v>3324752135</v>
       </c>
       <c r="N75" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O75" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P75" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q75" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R75" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S75" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="T75" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U75" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A76" s="2">
         <v>75</v>
       </c>
@@ -4966,33 +4995,33 @@
         <v>9674645471</v>
       </c>
       <c r="N76" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O76" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P76" s="10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Q76" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R76" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S76" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="T76" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U76" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="77" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A77" s="2">
         <v>76</v>
       </c>
@@ -5003,33 +5032,33 @@
         <v>9073681886</v>
       </c>
       <c r="N77" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O77" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P77" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q77" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R77" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S77" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="T77" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U77" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="78" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="2">
         <v>77</v>
       </c>
@@ -5047,33 +5076,33 @@
         <v>3324316997</v>
       </c>
       <c r="N78" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O78" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P78" s="10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Q78" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R78" s="10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="S78" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="T78" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U78" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="79" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="2">
         <v>78</v>
       </c>
@@ -5091,33 +5120,33 @@
         <v>3322291779</v>
       </c>
       <c r="N79" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O79" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P79" s="10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Q79" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R79" s="10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="S79" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="T79" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U79" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="80" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="2">
         <v>79</v>
       </c>
@@ -5135,33 +5164,33 @@
         <v>3323215151</v>
       </c>
       <c r="N80" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O80" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P80" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q80" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R80" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S80" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="T80" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U80" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="81" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A81" s="2">
         <v>80</v>
       </c>
@@ -5179,33 +5208,33 @@
         <v>3323342404</v>
       </c>
       <c r="N81" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O81" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P81" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Q81" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R81" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S81" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="T81" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U81" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="82" spans="1:21" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A82" s="2">
         <v>81</v>
       </c>
@@ -5219,33 +5248,33 @@
         <v>169</v>
       </c>
       <c r="N82" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O82" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P82" s="10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Q82" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R82" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S82" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="T82" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U82" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="83" spans="1:21" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A83" s="2">
         <v>82</v>
       </c>
@@ -5259,33 +5288,33 @@
         <v>171</v>
       </c>
       <c r="N83" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O83" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P83" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q83" s="10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R83" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S83" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="T83" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U83" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="84" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="2">
         <v>83</v>
       </c>
@@ -5299,33 +5328,33 @@
         <v>9606279184</v>
       </c>
       <c r="N84" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O84" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P84" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Q84" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R84" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S84" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="T84" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U84" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="85" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="2">
         <v>84</v>
       </c>
@@ -5343,33 +5372,33 @@
         <v>8777867589</v>
       </c>
       <c r="N85" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O85" s="10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P85" s="10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Q85" s="10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R85" s="10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="S85" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="T85" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U85" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="86" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A86" s="2">
         <v>85</v>
       </c>
@@ -5383,33 +5412,33 @@
         <v>8017672075</v>
       </c>
       <c r="N86" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O86" s="10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P86" s="10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Q86" s="10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R86" s="10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="S86" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="T86" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U86" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="87" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A87" s="2">
         <v>86</v>
       </c>
@@ -5423,33 +5452,33 @@
         <v>3324492810</v>
       </c>
       <c r="N87" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O87" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P87" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q87" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R87" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S87" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="T87" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U87" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="88" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A88" s="2">
         <v>87</v>
       </c>
@@ -5467,33 +5496,33 @@
         <v>3324967196</v>
       </c>
       <c r="N88" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O88" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P88" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q88" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R88" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S88" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="T88" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U88" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="89" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A89" s="2">
         <v>88</v>
       </c>
@@ -5511,33 +5540,33 @@
         <v>9830701347</v>
       </c>
       <c r="N89" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O89" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P89" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Q89" s="10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R89" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S89" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="T89" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U89" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="90" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A90" s="2">
         <v>89</v>
       </c>
@@ -5551,33 +5580,33 @@
         <v>3324961723</v>
       </c>
       <c r="N90" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O90" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P90" s="10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Q90" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R90" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S90" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="T90" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U90" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="91" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A91" s="2">
         <v>90</v>
       </c>
@@ -5595,33 +5624,33 @@
         <v>9007792852</v>
       </c>
       <c r="N91" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O91" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P91" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Q91" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R91" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S91" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="T91" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U91" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="92" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A92" s="2">
         <v>91</v>
       </c>
@@ -5635,33 +5664,33 @@
         <v>8902765583</v>
       </c>
       <c r="N92" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O92" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P92" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Q92" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R92" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S92" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="T92" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U92" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="93" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A93" s="2">
         <v>92</v>
       </c>
@@ -5675,33 +5704,33 @@
         <v>9331866252</v>
       </c>
       <c r="N93" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O93" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P93" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Q93" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R93" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S93" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="T93" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U93" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="94" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A94" s="2">
         <v>93</v>
       </c>
@@ -5715,33 +5744,33 @@
         <v>9903540099</v>
       </c>
       <c r="N94" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O94" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P94" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Q94" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R94" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S94" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="T94" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U94" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="95" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A95" s="2">
         <v>94</v>
       </c>
@@ -5755,33 +5784,33 @@
         <v>8336998663</v>
       </c>
       <c r="N95" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O95" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P95" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Q95" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R95" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S95" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="T95" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U95" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="96" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A96" s="2">
         <v>95</v>
       </c>
@@ -5795,33 +5824,33 @@
         <v>9339527506</v>
       </c>
       <c r="N96" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O96" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P96" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q96" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R96" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S96" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="T96" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U96" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="97" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A97" s="2">
         <v>96</v>
       </c>
@@ -5832,33 +5861,33 @@
         <v>9903312630</v>
       </c>
       <c r="N97" s="10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O97" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P97" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q97" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R97" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S97" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="T97" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U97" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="98" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A98" s="2">
         <v>97</v>
       </c>
@@ -5869,33 +5898,33 @@
         <v>9836747400</v>
       </c>
       <c r="N98" s="10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O98" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P98" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Q98" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R98" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S98" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="T98" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U98" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="99" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A99" s="2">
         <v>98</v>
       </c>
@@ -5906,33 +5935,33 @@
         <v>8100188019</v>
       </c>
       <c r="N99" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O99" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P99" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q99" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R99" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S99" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="T99" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U99" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="100" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A100" s="2">
         <v>99</v>
       </c>
@@ -5943,33 +5972,33 @@
         <v>197</v>
       </c>
       <c r="N100" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O100" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P100" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q100" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R100" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S100" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="T100" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U100" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="101" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A101" s="2">
         <v>100</v>
       </c>
@@ -5980,33 +6009,33 @@
         <v>198</v>
       </c>
       <c r="N101" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O101" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P101" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Q101" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R101" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S101" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="T101" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U101" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="102" spans="1:21" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A102" s="2">
         <v>101</v>
       </c>
@@ -6017,33 +6046,33 @@
         <v>201</v>
       </c>
       <c r="N102" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O102" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P102" s="10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Q102" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R102" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S102" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="T102" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U102" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="103" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A103" s="2">
         <v>102</v>
       </c>
@@ -6054,33 +6083,33 @@
         <v>202</v>
       </c>
       <c r="N103" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O103" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P103" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Q103" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R103" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S103" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="T103" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U103" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="104" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A104" s="2">
         <v>103</v>
       </c>
@@ -6091,33 +6120,33 @@
         <v>203</v>
       </c>
       <c r="N104" s="10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O104" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P104" s="10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Q104" s="10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R104" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S104" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="T104" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U104" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="105" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A105" s="2">
         <v>104</v>
       </c>
@@ -6128,33 +6157,33 @@
         <v>204</v>
       </c>
       <c r="N105" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O105" s="10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P105" s="10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Q105" s="10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R105" s="10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="S105" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="T105" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U105" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="106" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A106" s="2">
         <v>105</v>
       </c>
@@ -6165,33 +6194,33 @@
         <v>205</v>
       </c>
       <c r="N106" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O106" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P106" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Q106" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R106" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S106" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="T106" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U106" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="107" spans="1:21" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A107" s="2">
         <v>106</v>
       </c>
@@ -6202,33 +6231,33 @@
         <v>206</v>
       </c>
       <c r="N107" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O107" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P107" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q107" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R107" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S107" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="T107" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U107" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="108" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A108" s="2">
         <v>107</v>
       </c>
@@ -6239,33 +6268,33 @@
         <v>208</v>
       </c>
       <c r="N108" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O108" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P108" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Q108" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R108" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S108" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="T108" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U108" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="109" spans="1:21" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A109" s="2">
         <v>108</v>
       </c>
@@ -6276,33 +6305,33 @@
         <v>210</v>
       </c>
       <c r="N109" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O109" s="10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P109" s="10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Q109" s="10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R109" s="10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="S109" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="T109" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="U109" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="110" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A110" s="2">
         <v>109</v>
       </c>
@@ -6313,33 +6342,33 @@
         <v>213</v>
       </c>
       <c r="N110" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O110" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P110" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q110" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R110" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S110" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="T110" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U110" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="111" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A111" s="2">
         <v>110</v>
       </c>
@@ -6350,33 +6379,33 @@
         <v>215</v>
       </c>
       <c r="N111" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O111" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P111" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Q111" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R111" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S111" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="T111" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U111" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="112" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A112" s="2">
         <v>111</v>
       </c>
@@ -6387,33 +6416,33 @@
         <v>217</v>
       </c>
       <c r="N112" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O112" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P112" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Q112" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R112" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S112" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="T112" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U112" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="113" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A113" s="2">
         <v>112</v>
       </c>
@@ -6424,33 +6453,33 @@
         <v>219</v>
       </c>
       <c r="N113" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O113" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P113" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q113" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R113" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S113" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="T113" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U113" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="114" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A114" s="2">
         <v>113</v>
       </c>
@@ -6461,33 +6490,33 @@
         <v>221</v>
       </c>
       <c r="N114" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O114" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P114" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Q114" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R114" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S114" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="T114" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U114" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="115" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A115" s="2">
         <v>114</v>
       </c>
@@ -6498,33 +6527,33 @@
         <v>223</v>
       </c>
       <c r="N115" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O115" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P115" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Q115" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R115" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S115" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="T115" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U115" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="116" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A116" s="2">
         <v>115</v>
       </c>
@@ -6535,33 +6564,33 @@
         <v>225</v>
       </c>
       <c r="N116" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O116" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P116" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q116" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R116" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S116" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="T116" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U116" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="117" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A117" s="2">
         <v>116</v>
       </c>
@@ -6572,33 +6601,33 @@
         <v>227</v>
       </c>
       <c r="N117" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O117" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P117" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Q117" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R117" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S117" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="T117" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U117" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="118" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A118" s="2">
         <v>117</v>
       </c>
@@ -6609,33 +6638,33 @@
         <v>229</v>
       </c>
       <c r="N118" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O118" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P118" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Q118" s="10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R118" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S118" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="T118" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U118" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="119" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A119" s="2">
         <v>118</v>
       </c>
@@ -6672,7 +6701,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="120" spans="1:21" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A120" s="2">
         <v>119</v>
       </c>
@@ -6709,7 +6738,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="121" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A121" s="2">
         <v>120</v>
       </c>
@@ -6746,7 +6775,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="122" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A122" s="2">
         <v>121</v>
       </c>
@@ -6790,7 +6819,7 @@
       <formula1>"Initial,Potential,Customer,Support,Upsells,Reject,Not-Contacted,Ex-Customer"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1:M1048576" xr:uid="{2B1A7696-043D-48CA-AA07-994E1107EEC6}">
-      <formula1>"Rahul Dutta,Sayan Basak,Anirban Chakraborty"</formula1>
+      <formula1>"Rahul Dutta,Sayan Basak,Anirban Chakraborty,Debashish Nath"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
@@ -6859,17 +6888,17 @@
       <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.86328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.86328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B1" s="15"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>249</v>
       </c>
@@ -6880,7 +6909,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="13">
         <v>1</v>
       </c>
@@ -6891,7 +6920,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="13">
         <v>2</v>
       </c>
@@ -6902,7 +6931,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
         <v>3</v>
       </c>
@@ -6913,7 +6942,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
         <v>4</v>
       </c>
@@ -6924,7 +6953,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="13">
         <v>5</v>
       </c>
@@ -6935,7 +6964,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="13">
         <v>6</v>
       </c>
@@ -6946,7 +6975,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="13">
         <v>7</v>
       </c>
@@ -6957,7 +6986,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="13">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
AI schools for workshop checked in
AI schools for workshop checked in
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Marketing/AI marketing/AI Workshop Schools.xlsx
+++ b/Offline/BusinessManagement/Marketing/AI marketing/AI Workshop Schools.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Marketing\AI marketing\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{988F82BF-22C1-4DB4-9585-2D5848F413D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="540" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="8" r:id="rId1"/>
@@ -19,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'School-Details'!$A$1:$U$122</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,13 +39,13 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>del</author>
     <author>User</author>
   </authors>
   <commentList>
-    <comment ref="J1" authorId="0" shapeId="0">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -68,7 +69,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L28" authorId="1" shapeId="0">
+    <comment ref="L28" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -975,7 +976,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1185,14 +1186,14 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1474,11 +1475,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:L24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1501,18 +1502,18 @@
         <v>121</v>
       </c>
       <c r="J2" s="14"/>
-      <c r="K2" s="27" t="s">
+      <c r="K2" s="28" t="s">
         <v>210</v>
       </c>
-      <c r="L2" s="28"/>
+      <c r="L2" s="29"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C3" s="16" t="s">
         <v>246</v>
       </c>
       <c r="D3" s="16">
-        <f>SUM('School-Details'!K:K)/D2</f>
-        <v>8.2644628099173556E-3</v>
+        <f>ROUND(SUM('School-Details'!K:K)/D2,2)</f>
+        <v>0.01</v>
       </c>
       <c r="J3" s="21" t="s">
         <v>269</v>
@@ -1875,14 +1876,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U122"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D38" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="I110" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J26" sqref="J26"/>
+      <selection pane="bottomRight" activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3017,7 +3018,7 @@
       <c r="F28" s="7" t="s">
         <v>290</v>
       </c>
-      <c r="J28" s="29">
+      <c r="J28" s="27">
         <v>45300</v>
       </c>
       <c r="K28" s="1">
@@ -4242,7 +4243,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="57" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -4286,7 +4287,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="58" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -4550,7 +4551,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="64" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <v>63</v>
       </c>
@@ -4638,7 +4639,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="66" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
         <v>65</v>
       </c>
@@ -4682,7 +4683,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="67" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
         <v>66</v>
       </c>
@@ -4726,7 +4727,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="68" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <v>67</v>
       </c>
@@ -4902,7 +4903,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="72" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A72" s="2">
         <v>71</v>
       </c>
@@ -4990,7 +4991,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="74" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A74" s="2">
         <v>73</v>
       </c>
@@ -6906,68 +6907,68 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:U122"/>
+  <autoFilter ref="A1:U122" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U1:U1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U1:U1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Initial,Potential,Customer,Support,Upsells,Reject,Not-Contacted,Ex-Customer"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1:M1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1:M1048576" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Rahul Dutta,Sayan Basak,Anirban Chakraborty,Debashish Nath"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="D31" r:id="rId1"/>
-    <hyperlink ref="D32" r:id="rId2"/>
-    <hyperlink ref="F7" r:id="rId3" display="https://www.google.com/search?q=panchasayar+siksha+niketan&amp;sca_esv=593615924&amp;rlz=1C1CHBF_enAU1047AU1047&amp;sxsrf=AM9HkKnlKkWvrpmDIvMzNnJR8ZC_8s6gNQ%3A1703524925488&amp;ei=PbqJZaauHY2KnesPo--TuAo&amp;gs_ssp=eJzj4tFP1zc0MqnMzTa1TDNgtFI1qDBONDAyNzRPNU1LM0xOTkuyAgqZpJmZmJgnGZgZGSWnpSV5SRUk5iVnJBYnViYWKRRnZhdnJCrkZWanliTmAQC7Qxln&amp;oq=panchasayar+s&amp;gs_lp=Egxnd3Mtd2l6LXNlcnAiDXBhbmNoYXNheWFyIHMqAggAMhQQLhivARjHARimAxioAxiABBiOBTIFEAAYgAQyBRAAGIAEMgsQLhiABBioAxidAzIFEAAYgAQyBRAAGIAEMgUQABiABDIFEAAYgAQyCBAAGIAEGMsBMggQABiABBjLATIjEC4YrwEYxwEYpgMYqAMYgAQYjgUYlwUY3AQY3gQY4ATYAQNIuzhQmhhYmCVwAXgBkAEAmAGvAqAB1gSqAQUyLTEuMbgBAcgBAPgBAcICChAAGEcY1gQYsAPCAg0QABiABBiKBRhDGLADwgIcEC4YgAQYigUYQxjHARivARjIAxiwAxiOBdgBAcICGRAuGIAEGIoFGEMYxwEYrwEYyAMYsAPYAQHCAg4QABjkAhjWBBiwA9gBAsICEBAuGEMYnQMYqAMYgAQYigXCAhAQLhiABBiKBRhDGKgDGJ0DwgIWEC4YQxivARjHARimAxioAxiABBiKBcICChAAGIAEGBQYhwLCAh8QLhhDGJ0DGKgDGIAEGIoFGJcFGNwEGN4EGOAE2AED4gMEGAAgQYgGAZAGDroGBggBEAEYCLoGBggCEAEYCboGBggDEAEYFA&amp;sclient=gws-wiz-serp"/>
-    <hyperlink ref="F8" r:id="rId4" display="https://www.google.com/search?q=miranda+high+school&amp;sca_esv=593615924&amp;rlz=1C1CHBF_enAU1047AU1047&amp;sxsrf=AM9HkKmR8dFtasrVNGZkMFIxGz5Wq06ZjA%3A1703525037148&amp;ei=rbqJZczSCOCWjuMPsMy_8AM&amp;oq=miranda+high+&amp;gs_lp=Egxnd3Mtd2l6LXNlcnAiDW1pcmFuZGEgaGlnaCAqAggAMg0QABiABBgUGIcCGMkDMgUQABiABDILEAAYgAQYigUYkgMyBRAAGIAEMgUQABiABDIKEAAYgAQYFBiHAjIFEAAYgAQyBRAAGIAEMgUQABiABDIFEAAYgARI7RNQ6AZY6AZwAXgAkAEAmAH0BqABuAyqAQM2LTK4AQHIAQD4AQHCAgoQABhHGNYEGLAD4gMEGAAgQYgGAZAGCA&amp;sclient=gws-wiz-serp&amp;lqi=ChNtaXJhbmRhIGhpZ2ggc2Nob29sSN-07OW4roCACForEAAQARACGAAYARgCIhNtaXJhbmRhIGhpZ2ggc2Nob29sKggIAhAAEAEQApIBBnNjaG9vbJoBI0NoWkRTVWhOTUc5blMwVkpRMEZuU1VOUGNqUnVSbVZuRUFFqgE7EAEyHhABIhpTQ3iPFiqMHHb-9vGb0lli1Rpc5Z8xE87GgDIXEAIiE21pcmFuZGEgaGlnaCBzY2hvb2w"/>
-    <hyperlink ref="D22" r:id="rId5"/>
-    <hyperlink ref="D25" r:id="rId6" display="mailto:official@younghorizonsschool.com"/>
-    <hyperlink ref="D26" r:id="rId7" display="mailto:iwanttojoin@siskol.edu.in"/>
-    <hyperlink ref="D27" r:id="rId8" display="mailto:lcgvm2012@gmail.com"/>
-    <hyperlink ref="D30" r:id="rId9"/>
-    <hyperlink ref="D33" r:id="rId10"/>
-    <hyperlink ref="D35" r:id="rId11"/>
-    <hyperlink ref="D37" r:id="rId12"/>
-    <hyperlink ref="D41" r:id="rId13"/>
-    <hyperlink ref="D42" r:id="rId14"/>
-    <hyperlink ref="D43" r:id="rId15"/>
-    <hyperlink ref="D47" r:id="rId16"/>
-    <hyperlink ref="D48" r:id="rId17"/>
-    <hyperlink ref="D49" r:id="rId18"/>
-    <hyperlink ref="D51" r:id="rId19"/>
-    <hyperlink ref="D52" r:id="rId20"/>
-    <hyperlink ref="D53" r:id="rId21"/>
-    <hyperlink ref="D54" r:id="rId22"/>
-    <hyperlink ref="D55" r:id="rId23"/>
-    <hyperlink ref="D56" r:id="rId24"/>
-    <hyperlink ref="D57" r:id="rId25"/>
-    <hyperlink ref="D58" r:id="rId26"/>
-    <hyperlink ref="D59" r:id="rId27"/>
-    <hyperlink ref="D60" r:id="rId28"/>
-    <hyperlink ref="D61" r:id="rId29"/>
-    <hyperlink ref="D62" r:id="rId30"/>
-    <hyperlink ref="D63" r:id="rId31"/>
-    <hyperlink ref="D64" r:id="rId32"/>
-    <hyperlink ref="D65" r:id="rId33"/>
-    <hyperlink ref="D66" r:id="rId34"/>
-    <hyperlink ref="D67" r:id="rId35"/>
-    <hyperlink ref="D68" r:id="rId36"/>
-    <hyperlink ref="D69" r:id="rId37"/>
-    <hyperlink ref="D70" r:id="rId38"/>
-    <hyperlink ref="D71" r:id="rId39"/>
-    <hyperlink ref="D72" r:id="rId40"/>
-    <hyperlink ref="D73" r:id="rId41"/>
-    <hyperlink ref="D75" r:id="rId42"/>
-    <hyperlink ref="D78" r:id="rId43"/>
-    <hyperlink ref="D79" r:id="rId44"/>
-    <hyperlink ref="D80" r:id="rId45"/>
-    <hyperlink ref="D81" r:id="rId46"/>
-    <hyperlink ref="D85" r:id="rId47"/>
-    <hyperlink ref="D88" r:id="rId48"/>
-    <hyperlink ref="D89" r:id="rId49"/>
-    <hyperlink ref="D91" r:id="rId50"/>
-    <hyperlink ref="D2" r:id="rId51"/>
-    <hyperlink ref="D28" r:id="rId52"/>
+    <hyperlink ref="D31" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="D32" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="F7" r:id="rId3" display="https://www.google.com/search?q=panchasayar+siksha+niketan&amp;sca_esv=593615924&amp;rlz=1C1CHBF_enAU1047AU1047&amp;sxsrf=AM9HkKnlKkWvrpmDIvMzNnJR8ZC_8s6gNQ%3A1703524925488&amp;ei=PbqJZaauHY2KnesPo--TuAo&amp;gs_ssp=eJzj4tFP1zc0MqnMzTa1TDNgtFI1qDBONDAyNzRPNU1LM0xOTkuyAgqZpJmZmJgnGZgZGSWnpSV5SRUk5iVnJBYnViYWKRRnZhdnJCrkZWanliTmAQC7Qxln&amp;oq=panchasayar+s&amp;gs_lp=Egxnd3Mtd2l6LXNlcnAiDXBhbmNoYXNheWFyIHMqAggAMhQQLhivARjHARimAxioAxiABBiOBTIFEAAYgAQyBRAAGIAEMgsQLhiABBioAxidAzIFEAAYgAQyBRAAGIAEMgUQABiABDIFEAAYgAQyCBAAGIAEGMsBMggQABiABBjLATIjEC4YrwEYxwEYpgMYqAMYgAQYjgUYlwUY3AQY3gQY4ATYAQNIuzhQmhhYmCVwAXgBkAEAmAGvAqAB1gSqAQUyLTEuMbgBAcgBAPgBAcICChAAGEcY1gQYsAPCAg0QABiABBiKBRhDGLADwgIcEC4YgAQYigUYQxjHARivARjIAxiwAxiOBdgBAcICGRAuGIAEGIoFGEMYxwEYrwEYyAMYsAPYAQHCAg4QABjkAhjWBBiwA9gBAsICEBAuGEMYnQMYqAMYgAQYigXCAhAQLhiABBiKBRhDGKgDGJ0DwgIWEC4YQxivARjHARimAxioAxiABBiKBcICChAAGIAEGBQYhwLCAh8QLhhDGJ0DGKgDGIAEGIoFGJcFGNwEGN4EGOAE2AED4gMEGAAgQYgGAZAGDroGBggBEAEYCLoGBggCEAEYCboGBggDEAEYFA&amp;sclient=gws-wiz-serp" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="F8" r:id="rId4" display="https://www.google.com/search?q=miranda+high+school&amp;sca_esv=593615924&amp;rlz=1C1CHBF_enAU1047AU1047&amp;sxsrf=AM9HkKmR8dFtasrVNGZkMFIxGz5Wq06ZjA%3A1703525037148&amp;ei=rbqJZczSCOCWjuMPsMy_8AM&amp;oq=miranda+high+&amp;gs_lp=Egxnd3Mtd2l6LXNlcnAiDW1pcmFuZGEgaGlnaCAqAggAMg0QABiABBgUGIcCGMkDMgUQABiABDILEAAYgAQYigUYkgMyBRAAGIAEMgUQABiABDIKEAAYgAQYFBiHAjIFEAAYgAQyBRAAGIAEMgUQABiABDIFEAAYgARI7RNQ6AZY6AZwAXgAkAEAmAH0BqABuAyqAQM2LTK4AQHIAQD4AQHCAgoQABhHGNYEGLAD4gMEGAAgQYgGAZAGCA&amp;sclient=gws-wiz-serp&amp;lqi=ChNtaXJhbmRhIGhpZ2ggc2Nob29sSN-07OW4roCACForEAAQARACGAAYARgCIhNtaXJhbmRhIGhpZ2ggc2Nob29sKggIAhAAEAEQApIBBnNjaG9vbJoBI0NoWkRTVWhOTUc5blMwVkpRMEZuU1VOUGNqUnVSbVZuRUFFqgE7EAEyHhABIhpTQ3iPFiqMHHb-9vGb0lli1Rpc5Z8xE87GgDIXEAIiE21pcmFuZGEgaGlnaCBzY2hvb2w" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="D22" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="D25" r:id="rId6" display="mailto:official@younghorizonsschool.com" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="D26" r:id="rId7" display="mailto:iwanttojoin@siskol.edu.in" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="D27" r:id="rId8" display="mailto:lcgvm2012@gmail.com" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="D30" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="D33" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="D35" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="D37" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
+    <hyperlink ref="D41" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
+    <hyperlink ref="D42" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
+    <hyperlink ref="D43" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink ref="D47" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
+    <hyperlink ref="D48" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
+    <hyperlink ref="D49" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
+    <hyperlink ref="D51" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
+    <hyperlink ref="D52" r:id="rId20" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
+    <hyperlink ref="D53" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
+    <hyperlink ref="D54" r:id="rId22" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
+    <hyperlink ref="D55" r:id="rId23" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
+    <hyperlink ref="D56" r:id="rId24" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
+    <hyperlink ref="D57" r:id="rId25" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
+    <hyperlink ref="D58" r:id="rId26" xr:uid="{00000000-0004-0000-0100-000019000000}"/>
+    <hyperlink ref="D59" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
+    <hyperlink ref="D60" r:id="rId28" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
+    <hyperlink ref="D61" r:id="rId29" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
+    <hyperlink ref="D62" r:id="rId30" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
+    <hyperlink ref="D63" r:id="rId31" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
+    <hyperlink ref="D64" r:id="rId32" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
+    <hyperlink ref="D65" r:id="rId33" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
+    <hyperlink ref="D66" r:id="rId34" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
+    <hyperlink ref="D67" r:id="rId35" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
+    <hyperlink ref="D68" r:id="rId36" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
+    <hyperlink ref="D69" r:id="rId37" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
+    <hyperlink ref="D70" r:id="rId38" xr:uid="{00000000-0004-0000-0100-000025000000}"/>
+    <hyperlink ref="D71" r:id="rId39" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
+    <hyperlink ref="D72" r:id="rId40" xr:uid="{00000000-0004-0000-0100-000027000000}"/>
+    <hyperlink ref="D73" r:id="rId41" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
+    <hyperlink ref="D75" r:id="rId42" xr:uid="{00000000-0004-0000-0100-000029000000}"/>
+    <hyperlink ref="D78" r:id="rId43" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
+    <hyperlink ref="D79" r:id="rId44" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
+    <hyperlink ref="D80" r:id="rId45" xr:uid="{00000000-0004-0000-0100-00002C000000}"/>
+    <hyperlink ref="D81" r:id="rId46" xr:uid="{00000000-0004-0000-0100-00002D000000}"/>
+    <hyperlink ref="D85" r:id="rId47" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
+    <hyperlink ref="D88" r:id="rId48" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
+    <hyperlink ref="D89" r:id="rId49" xr:uid="{00000000-0004-0000-0100-000030000000}"/>
+    <hyperlink ref="D91" r:id="rId50" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
+    <hyperlink ref="D2" r:id="rId51" xr:uid="{00000000-0004-0000-0100-000032000000}"/>
+    <hyperlink ref="D28" r:id="rId52" xr:uid="{00000000-0004-0000-0100-000033000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId53"/>
@@ -6976,7 +6977,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>